<commit_message>
Finishing up the report summary chain.
</commit_message>
<xml_diff>
--- a/outputs/analysis.xlsx
+++ b/outputs/analysis.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M93"/>
+  <dimension ref="A1:M94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,7 +503,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>4,5</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -528,12 +528,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>The document contains a comprehensive Information Security Policy detailing the scope, responsibilities, enforcement, and management commitment to information security based on ISO27001 standards.</t>
+          <t>Information Security Policy document defines baseline control measures, scope, enforcement, roles and responsibilities, and management commitment to information security aligned with ISO27001 standards.</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Information Security Policy [Internal].docx - Sections: Confidentiality Statement, Chapter 1 General, Section 1.1 Scope of the policy, Section 1.4 Enforcements</t>
+          <t>Information Security Policy [Internal].docx: 'This document details the policies and standards for the information security of Reducate... These policies will be based on ISO27001 standards.'; 'This policy will come into effect after approval by the director of Reducate.'; 'Chapter 1 General' and 'Section - 1.1 Scope of the policy'.</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
@@ -545,17 +545,17 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Information security policy is shared with all employees; information security goals are communicated and added to training; policy documentation is reviewed and updated as part of management review.</t>
+          <t>Information Security Policy is referenced as an internal document relevant to the meeting and shared with all employees; security objectives and measures are reviewed and updated regularly.</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Include explicit excerpts or summaries of the Information Security Policy document to strengthen evidence of baseline control measures and management commitment.</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>🟡</t>
         </is>
       </c>
     </row>
@@ -587,34 +587,34 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Acceptable use policies are defined in the Information Technology Acceptable Usage Policy, including rules on IT, email, internet use, and disciplinary actions for misuse.</t>
+          <t>Acceptable use policies for IT, email, internet, and mobile devices are defined with disciplinary measures for violations.</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Information Security Policy [Internal].docx - Chapter 5 Personnel Security - 5.1 Information Technology Acceptable Usage Policy</t>
+          <t>Information Security Policy [Internal].docx: '5.1 Information Technology Acceptable Usage Policy' and subsections including '5.1.3 IT Policy', '5.1.4 IT Security', '5.1.5 Personal Use of Company Facilities', and '5.1.11 Mobile equipment Usage'.</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>No explicit reference to acceptable use policies or disciplinary actions for misuse found in evidence text.</t>
+          <t>Disciplinary processes and training updates are discussed, implying enforcement of acceptable use policies.</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Include acceptable use policy documentation and evidence of enforcement.</t>
+          <t>Provide explicit acceptable use policies and disciplinary measures documentation.</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>🟡</t>
         </is>
       </c>
     </row>
@@ -642,12 +642,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Documented procedures exist for return of company assets upon termination of employment, including laptops, mobile phones, and other equipment.</t>
+          <t>Procedures for return of company assets at termination of employment are documented and enforced.</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Information Security Policy [Internal].docx - Section 2.4 Termination of employment</t>
+          <t>Information Security Policy [Internal].docx: 'Section - 2.4 Termination of employment' and 'Section - 2.1.2 Equipment usage' specify return of laptops, mobile phones, and other assets on last day of employment.</t>
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
@@ -659,7 +659,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Checklist includes 'Inleveren sleutel en tag' and 'Afmelden Office' and 'Computer deinstalleren' indicating documented procedures for return of assets upon termination.</t>
+          <t>Checklist for termination includes return of keys, office sign-off, and computer de-registration, indicating enforcement of asset return procedures.</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -701,34 +701,34 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Information classification schemes are prepared based on value, legal requirements, and handling caution. Asset owners classify and manage information assets accordingly.</t>
+          <t>Information classification schemes are established based on value, legal requirements, and handling caution.</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Information Security Policy [Internal].docx - Chapter 3 Management of Information - 3.1 Classification of information; Chapter 4 Asset Classification and Control</t>
+          <t>Information Security Policy [Internal].docx: 'Section - 3.1 Classification of information' and '4. Asset Classification and Control' describe classification schemes and responsibilities.</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>No explicit information classification scheme or asset owner responsibilities found in evidence text.</t>
+          <t>Information security objectives include data confidentiality and integrity, implying classification schemes, but no explicit classification scheme documentation found.</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Provide documented classification schemes and evidence of implementation.</t>
+          <t>Provide documented information classification schemes.</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>🟡</t>
         </is>
       </c>
     </row>
@@ -756,29 +756,29 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Information must be labelled and handled according to classification schemes. Guidelines for labelling and handling are provided.</t>
+          <t>Information assets are labelled and handled according to classification schemes with guidelines for labelling and handling.</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Information Security Policy [Internal].docx - Chapter 3 Management of Information - 3.2 Labelling and handling of information; Chapter 4 Asset Classification and Control - 4.1 Information Labelling and Handling</t>
+          <t>Information Security Policy [Internal].docx: 'Section - 3.2 Labelling and handling of information' and '4.1 Information Labelling and Handling' specify labelling and handling requirements.</t>
         </is>
       </c>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>No explicit evidence found in provided documents.</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>No explicit labelling guidelines or evidence of labelling information according to classification found.</t>
+          <t>No mention of labelling of information assets or guidelines for labelling and handling.</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Include labelling procedures and evidence of application.</t>
+          <t>Develop and document labelling procedures aligned with classification schemes.</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -815,24 +815,24 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Electronic messaging and information transfer are controlled and protected according to classification. External electronic communications require prior approval.</t>
+          <t>Information transfer is controlled with classification-based protection and approval for external electronic messaging.</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Information Security Policy [Internal].docx - Chapter 7 Security of Communication - 7.3 Electronic messaging; Chapter 5 Personnel Security - 5.1.1 Data Protection</t>
+          <t>Information Security Policy [Internal].docx: 'Section - 7.3 Electronic messaging' and '6.7 Electronic Messaging System Controls' describe protection of electronic messages and approval for external services.</t>
         </is>
       </c>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>No explicit controls or approvals for electronic messaging or information transfer found in evidence text.</t>
+          <t>Information transfer controls are implied in risk assessments and audit results but no explicit procedures or approvals for external electronic messaging are documented.</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -842,7 +842,7 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>🟡</t>
         </is>
       </c>
     </row>
@@ -870,29 +870,29 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Access control policies are defined, including user registration, de-registration, access restriction, privileged access management, and periodic audits.</t>
+          <t>Access control policies and procedures are established including user registration, access restriction, privileged access management, and periodic audits.</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Information Security Policy [Internal].docx - Chapter 5 Access Control; Chapter 7 Access Control policy</t>
+          <t>Information Security Policy [Internal].docx: 'Chapter 5 Access Control' sections 5.1 to 5.4 detail user registration, access restriction, privileged access, and user access management.</t>
         </is>
       </c>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
+          <t>Matrix rechten Zoho (Internal).pdf</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Centralised password manager 'Zoho Vault' implemented; audit results mention one remaining point concerning A.5.15; access rights and segregation of duties discussed in relation to Zoho rights.</t>
+          <t>Access rights and user roles are managed and documented within Zoho CRM and other systems; periodic audits are implied in management review.</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Clarify and resolve remaining audit points related to access control.</t>
+          <t>Include formal access control policy documents and audit reports.</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -925,34 +925,34 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>User identities are managed through formal registration and de-registration processes with unique user IDs and controls on shared or anonymous IDs.</t>
+          <t>Formal processes for user registration, de-registration, and unique user ID assignment are in place.</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Information Security Policy [Internal].docx - Chapter 5 Access Control - 5.1 User registration and de-registration; Chapter 7 Access Control policy - 7.1 Authentication</t>
+          <t>Information Security Policy [Internal].docx: 'Section - 5.1 User registration and de-registration' and '7.1 Authentication' specify identity management controls.</t>
         </is>
       </c>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>2.4.7 Template checklist indienst.PNG.pdf</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>No explicit user identity management process or registration/deregistration procedures found.</t>
+          <t>Checklist for onboarding includes account creation and system sign-up, indicating formal user registration processes.</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Provide documented identity management procedures.</t>
+          <t>Provide documented user registration and de-registration procedures.</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>🟡</t>
         </is>
       </c>
     </row>
@@ -980,12 +980,12 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Password policies and secret authentication information handling are defined, including password complexity, confidentiality, change management, and secure storage.</t>
+          <t>Password policies and controls for secret authentication information are defined and enforced.</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Information Security Policy [Internal].docx - Chapter 4 Management of Computers and Information Equipment - 4.1 Use of secret authentication information; Chapter 7 Access Control policy - 7.3 Password Policy</t>
+          <t>Information Security Policy [Internal].docx: 'Section - 4.1 Use of secret authentication information such as passwords' and '7.3 Password Policy' detail password management and authentication controls.</t>
         </is>
       </c>
       <c r="H10" t="inlineStr"/>
@@ -997,7 +997,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Password policies enforce minimum length (12-14 characters), complexity (uppercase, lowercase, numbers, special characters), password history, expiration (120-180 days), lockout after 10 failed attempts, and two-factor authentication enabled for all users.</t>
+          <t>Password policies enforce minimum length, complexity, history, expiration, lockout, and two-factor authentication for all users.</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -1035,34 +1035,34 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Access rights are assigned based on business needs with formal authorization, periodic review, and revocation upon termination or role change.</t>
+          <t>Access rights are assigned based on business needs with formal authorization and periodic review.</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Information Security Policy [Internal].docx - Chapter 5 Access Control - 5.1 User registration and de-registration; Chapter 7 Access Control policy - 7.2 Authorisation and Access Control; 7.4 User Access Management</t>
+          <t>Information Security Policy [Internal].docx: 'Section - 5.2 Information access restriction' and '7.2 Authorisation and Access Control' describe access rights management.</t>
         </is>
       </c>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
+          <t>Matrix rechten Zoho (Internal).pdf</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Access rights assigned based on business needs with formal authorization; periodic reviews discussed in management review; Zoho rights and financial system rights used for segregation of duties.</t>
+          <t>Access rights are assigned based on roles with formal authorization; changes are tracked and reviewed.</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Include evidence of periodic access rights review documentation.</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>🟡</t>
         </is>
       </c>
     </row>
@@ -1094,12 +1094,12 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Contracts and SLAs with external service providers are required, including verification of credentials, NDA agreements, access control, and security policy awareness.</t>
+          <t>Supplier relationships are managed with contracts, SLAs, credential verification, NDA requirements, access control, and ongoing contract management.</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Information Security Policy [Internal].docx - Chapter 3 Business partnership and Outsourcing</t>
+          <t>Information Security Policy [Internal].docx: '3. Business partnership and Outsourcing' sections 3.1 to 3.3 detail supplier security requirements and contract management.</t>
         </is>
       </c>
       <c r="H12" t="inlineStr"/>
@@ -1111,17 +1111,17 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Third-party management is operating effectively; vendor risk assessments are performed; third-party register is up to date; contracts and audits are reviewed.</t>
+          <t>Vendor risk assessments and contract management are discussed; third-party register is maintained and reviewed.</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Provide supplier contracts including information security clauses and SLAs.</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>🟡</t>
         </is>
       </c>
     </row>
@@ -1153,12 +1153,12 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Roles and responsibilities are clearly defined for CEO, ISSC, ISWG, Operational Directors, IT Asset Managers, Managers, Users, and Executive responsibilities with competencies and duties outlined.</t>
+          <t>Clear assignment of roles and responsibilities for information security including CEO, ISSC, Operational Director, IT Asset Managers, Managers, Users, and committees (ISSC, ISWG).</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Information Security Policy [Internal].docx - Section 1.5 Roles and Responsibilities</t>
+          <t>Information Security Policy [Internal].docx: 'Section - 1.5 Roles and Responsibilities' and '2. Security Organisation' sections detailing roles such as CEO, ISSC, ISWG, IT Asset Managers, Managers, Users.</t>
         </is>
       </c>
       <c r="H13" t="inlineStr"/>
@@ -1170,17 +1170,17 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Attendees list includes Managing Director, ISMS Responsible, System Administrator, Finance Manager, and Project Manager, indicating defined roles; responsibilities discussed in meeting; roles such as ISSC and ISWG referenced throughout.</t>
+          <t>Attendees list includes CEO, ISMS Responsible, System Administrator, Finance Manager, and Project Manager, indicating clear assignment of roles and responsibilities for information security.</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Provide documented role descriptions or responsibility matrices to further clarify assignments.</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>🟡</t>
         </is>
       </c>
     </row>
@@ -1212,12 +1212,12 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Supplier agreements and contracts with external service providers must include security requirements, risk assessments before contract signing, and clauses for compliance with Reducate's security policy.</t>
+          <t>Supplier agreements and contracts must include information security requirements and risk assessments before signing. Contracts must cover scope, roles, SLAs, access control, incident handling, change management, audits, data protection, and termination.</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Section 3.1 Business Partnership Security; 3.1.3 All outsourcing to External Service Providers must be formalised through a contract; 3.1.5 External Service Providers must be made aware of relevant parts of Reducate security policy; 3.3 Business Partnership Contracts; 3.3.1 Contract clauses including access control, incident handling, change management, audits, data protection; 3.3.2 Contract management responsibilities. (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx, Section 3.3 Business Partnership Contracts (pages 20-22): 'Before the contract is signed... risk reducing controls... must be incorporated...'; 'Contracts must address... access control mechanisms, IT Incident &amp; Problem handling process, IT Change management process, periodic audits, data protection.'</t>
         </is>
       </c>
       <c r="H14" t="inlineStr"/>
@@ -1229,17 +1229,17 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Supplier contracts include security requirements; risk assessments before contract signing discussed; compliance with Reducate's security policy monitored.</t>
+          <t>Contracts and risk assessments are part of vendor management; however, no explicit contract clauses or risk assessment documents are provided.</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Include sample contracts with security requirements and risk assessment reports.</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>🟡</t>
         </is>
       </c>
     </row>
@@ -1271,12 +1271,12 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>ICT supply chain risks are managed by verifying credentials of external service providers, maintaining a list of key IT suppliers, and ensuring compliance with security policies and contracts.</t>
+          <t>Credentials of external service providers must be verified; NDAs signed; access authorized and limited; network connectivity controlled; key suppliers maintained and reviewed annually.</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Section 3.1.1 Credentials of potential External Service Providers must be verified; 3.1.9 Key IT-suppliers list maintained and reviewed yearly; 5.1.1 Data Protection and GDPR compliance with external vendors; 3.1 Business Partnership Security (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx, Section 3.1 Business Partnership Security and 3.2 Non-Disclosure Agreements (pages 19-20): 'Credentials of potential External Service Providers must be verified'; 'All External Service Providers must sign NDA'; 'Access must be authorised'; 'Network connectivity must comply with policies'; 'Key IT-suppliers list maintained and reviewed yearly.'</t>
         </is>
       </c>
       <c r="H15" t="inlineStr"/>
@@ -1288,17 +1288,17 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>ICT supply chain risks managed by verifying credentials of external service providers; key IT suppliers list maintained; compliance ensured.</t>
+          <t>Credential verification and NDA requirements for external providers are mentioned in vendor risk assessments.</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Provide documented evidence of NDA signings and access authorizations.</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>🟡</t>
         </is>
       </c>
     </row>
@@ -1330,12 +1330,12 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Supplier contracts are managed by responsible persons with periodic reviews of performance using SLA metrics, quality, timeliness, communication, compliance, and security posture.</t>
+          <t>Contracts include periodic audits and performance reviews; a responsible person manages contracts; change management processes are in place for IT infrastructure and services.</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Section 3.3.2 Contract Management - responsible person allocated; periodic reviews on performance using SLA metrics and other indicators; 3.3 Business Partnership Contracts (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx, Section 3.3.2 Contract Management (page 21): 'Responsible person allocated for contract management'; 'Periodic reviews on performance including SLA metrics, quality, timeliness, compliance'; Section 6.2 Operational change control (page 33): 'Changes to information processing facilities and systems should be controlled with formal management responsibilities and procedures.'</t>
         </is>
       </c>
       <c r="H16" t="inlineStr"/>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Supplier contracts managed by responsible persons; periodic reviews of performance using SLA metrics, quality, timeliness, communication, compliance, and security posture.</t>
+          <t>Contract management includes periodic audits and performance reviews; change management processes are in place.</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
@@ -1389,34 +1389,34 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Use of cloud services must be approved by IT-Manager and ISWG; access restricted per access control policies; yearly review of files shared externally; encryption and secure communication protocols enforced.</t>
+          <t>Use of cloud services must be approved by IT-Manager and ISWG; access restricted per access control policies; cloud applications must use TLS 1.2 or higher; annual security testing of TLS; cloud email services preferred.</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Section 7.5 Guideline for Usage of Public Cloud Services; 4.1.3 Reporting Information Assets - yearly review of files shared externally; 10.5 Cloud applications must have TLS 1.2 or higher; 10.6 Yearly TLS security test; 10.7 Approved SSL providers; 5.1.1 Data Protection and GDPR compliance; 5.1.4 File sharing only via approved directories (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx, Section 7.5 Guideline for Usage of Public Cloud Services (page 38): 'Use of any Cloud based applications and/or services must be approved'; Section 10 Cryptography (page 52): 'Cloud applications must have minimum TLS 1.2 or higher'; Section 6.7 Electronic Messaging System Controls (page 44): 'Use Google mail or other cloud email services.'</t>
         </is>
       </c>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>No explicit approval process or yearly review of cloud services found in evidence text.</t>
+          <t>Cloud service use requires approval by IT Manager and ISWG; TLS 1.2+ usage and annual security testing are mentioned.</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Document cloud service approval and review procedures.</t>
+          <t>Provide documented cloud service approval records and test reports.</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>🟡</t>
         </is>
       </c>
     </row>
@@ -1448,12 +1448,12 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Incident management procedures are established including monitoring, detection, analysis, reporting, assessment, handling, recovery, and reporting to parent companies; IT Security function maintains subscriptions to vulnerability notifications; monthly ISSC incident briefings.</t>
+          <t>Incident response procedures established covering monitoring, detection, analysis, reporting, recovery, and communication; IT Security function responsible; incident logs maintained; CAPA forms used; incident response plan included in Business Continuity Plan.</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Chapter 9 Management of Information Security Incidents; Section 9.1 Responsibilities and procedures; 6.5 Security incident management; 6.5.1 to 6.5.7 detailed incident management controls; monthly ISSC briefings; Appendix - 6.5 Security incident management (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx, Section 6.5 Security incident management (pages 34-36): 'Security Incident management responsibilities and procedures established'; 'Incident response policy implemented'; 'Procedures for monitoring, detecting, analysing, reporting'; 'CAPA forms used'; Business Continuity Plan E-WISE [Restricted].docx.pdf, Appendix 1 Incident Response Plan (pages 11-12).</t>
         </is>
       </c>
       <c r="H18" t="inlineStr"/>
@@ -1465,7 +1465,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Incident management procedures established; IT Security function maintains subscriptions to vulnerability notifications; monthly ISSC incident briefings include incident discussions.</t>
+          <t>Incident response procedures and logs are maintained; CAPA forms used; incident response plan included in Business Continuity Plan.</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1507,12 +1507,12 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Procedures exist for assessment and classification of information security events as incidents; IT Security function analyzes incidents and uses CAPA forms; decisions on incident classification and response are documented.</t>
+          <t>Procedures for assessment and classification of information security events as incidents; IT Security function analyses and identifies causes; decisions on incident classification and escalation made by designated roles.</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Chapter 9 Section 9.1(b) Procedures for assessment and decision of information security events; 6.5.5 Procedures to analyze and identify cause of incidents; CAPA forms usage; 6.5.6 Documentation and review of emergency actions; Appendix - 6.5 Security incident management (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx, Section 6.5 Security incident management (page 35): 'Procedures for assessment and decision of information security events'; 'IT Security function analyses and identifies cause'; 'All significant incidents briefed to ISSC monthly.'</t>
         </is>
       </c>
       <c r="H19" t="inlineStr"/>
@@ -1524,7 +1524,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Procedures exist for assessment and classification of information security events; CAPA forms used; incident analysis and documentation performed.</t>
+          <t>Procedures for assessment and classification of incidents are discussed; IT Security function analyses causes and escalates incidents.</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -1566,12 +1566,12 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Incident response procedures include containment, eradication, recovery, reporting to ISSC and parent companies; emergency actions documented and reviewed; users instructed to report incidents promptly.</t>
+          <t>Incident handling procedures include containment, eradication, recovery; emergency actions documented and reviewed; communication responsibilities defined; incident response plan activated automatically.</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Chapter 9 Section 9.1(c) Procedures for handling information security incidents; 6.5.1 to 6.5.7 Security incident management; 5.1.4 Users must report security violations immediately; Appendix - 6.5 Security incident management (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx, Section 6.5 Security incident management (pages 35-36): 'Emergency actions documented and reviewed'; Business Continuity Plan E-WISE [Restricted].docx.pdf, Section 2.4 Plan activation; plan deactivation (page 6): 'Incident Response Plan activated automatically on incident.'</t>
         </is>
       </c>
       <c r="H20" t="inlineStr"/>
@@ -1583,7 +1583,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Incident response procedures include containment, eradication, recovery, reporting to ISSC and parent companies; emergency actions documented and reviewed; users instructed to report incidents promptly.</t>
+          <t>Incident handling procedures include containment, eradication, recovery; communication responsibilities defined; plan activated automatically.</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -1625,12 +1625,12 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Yearly simulations and reviews of incidents are conducted; CAPA forms used to document corrective actions; ISSC reviews incidents and takes remediation actions; lessons learned incorporated into ISMS.</t>
+          <t>Incident reviews and lessons learned incorporated; CAPA forms used; incident reports reviewed by ISSC; restoration and resumption plans developed post-incident.</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>6.5.5 Incident analysis and cause identification; yearly simulation recommended; 6.5.6 Documentation and review with ISSC or ISWG; 5.1.2 Data incidents and GDPR improvements discussed biannually; Chapter 10 Section 10.1 Review of information security; Appendix - 6.5 Security incident management (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx, Section 6.5 Security incident management (page 36): 'CAPA forms used to describe analysis'; 'All emergency actions reviewed with ISSC or ISWG'; Business Continuity Plan E-WISE [Restricted].docx.pdf, Chapter 3 Restoring and resuming business activities (pages 9-10).</t>
         </is>
       </c>
       <c r="H21" t="inlineStr"/>
@@ -1642,7 +1642,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Yearly simulations and reviews of incidents conducted; CAPA forms used for corrective actions; ISSC reviews incidents and takes remediation actions; lessons learned incorporated into ISMS.</t>
+          <t>Incident reviews and lessons learned incorporated; CAPA forms used; incident reports reviewed by ISSC; restoration plans developed.</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
@@ -1684,12 +1684,12 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Evidence collection procedures include audit trails, issue tracking, documentation of incident steps; evidence retained for analysis, reporting, and reconstruction; CAPA forms used.</t>
+          <t>Procedures include collection and preservation of evidence such as audit trails; documentation of incident handling steps; evidence captured in issue tracking tools.</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>6.5.5 Collection of evidence such as audit trails; all evidence captured in issue tracking tool; documentation of emergency actions; Appendix - 6.5 Security incident management (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx, Section 6.5 Security incident management (page 36): 'Collection of evidence such as audit trails'; 'All evidence captured in issue tracking tool to ensure analysis, reporting and reconstruction.'</t>
         </is>
       </c>
       <c r="H22" t="inlineStr"/>
@@ -1701,17 +1701,17 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>CAPA made and improvement implemented regarding evidence collection in incident procedures; audit trails and documentation referenced.</t>
+          <t>CAPA made and improvement implemented for evidence collection in incident procedures; incident logs maintained.</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Provide detailed procedures for evidence collection and preservation.</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>🟡</t>
         </is>
       </c>
     </row>
@@ -1739,12 +1739,12 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Business Continuity Plan defines management of incidents and recovery within deadlines; preservation of damaged assets; assessment and action plans; communication and resource allocation during disruptions.</t>
+          <t>Business Continuity Plan defines management of incidents and recovery within deadlines; resources and communication plans defined; order of recovery and interdependencies documented.</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Business Continuity Plan E-WISE [Restricted].docx.pdf; Chapter 2 Business Continuity Plan; Sections 2.1 to 3.3; Incident Response Plan; Disaster Recovery Plan; Communication; Resource management; Preservation of damaged assets; Action plans (Business Continuity Plan E-WISE [Restricted].docx.pdf)</t>
+          <t>Business Continuity Plan E-WISE [Restricted].docx.pdf, Chapter 2 Business Continuity Plan (pages 4-9): 'Defines how E-WISE will manage incidents and recover activities'; 'Order of recovery for activities'; 'Communication plans and resources defined.'</t>
         </is>
       </c>
       <c r="H23" t="inlineStr"/>
@@ -1756,7 +1756,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Business Continuity Plan includes restore tests; restore tests successfully done; requirements for restore tests to be updated in 2025.</t>
+          <t>Business Continuity Plan defines incident management and recovery within deadlines; restore tests successfully done and planned updates noted.</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
@@ -1798,12 +1798,12 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Segregation of duties is mandated when assigning responsibilities, with additional controls such as monitoring and audit trails recommended where segregation is difficult.</t>
+          <t>Segregation of duties is ensured when assigning responsibilities to reduce risk of misuse; monitoring and audit trails are considered where segregation is difficult.</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Information Security Policy [Internal].docx - Section 1.5 Roles and Responsibilities; Chapter 6 IT Operations Controls - 6.4 Segregation of Duties</t>
+          <t>Information Security Policy [Internal].docx: 'Section - 2.1.5 Change of employment' and '6.4 Segregation of Duties' - 'Reducate and group companies management must ensure segregation of duties when assigning responsibilities.'</t>
         </is>
       </c>
       <c r="H24" t="inlineStr"/>
@@ -1815,17 +1815,17 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Segregation of duties is determined based on Zoho rights and financial system rights; risk mapping has been redone to address segregation of duties issues.</t>
+          <t>Segregation of duties is addressed in audit results and risk mapping, specifically mentioning segregation based on Zoho rights and financial system rights.</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Include formal documented procedures or controls demonstrating segregation of duties in practice.</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>🟡</t>
         </is>
       </c>
     </row>
@@ -1853,34 +1853,34 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Business Continuity Plan includes Disaster Recovery Plans for IT infrastructure and services; recovery time objectives defined; resources and responsibilities assigned; restoration and resumption steps detailed.</t>
+          <t>Disaster Recovery Plans for IT infrastructure and services included; resources and recovery time objectives defined; restoration and resumption procedures documented.</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Business Continuity Plan E-WISE [Restricted].docx.pdf; Chapter 2 Sections 2.1 to 3.3; Appendix 6 Disaster Recovery Plans; Recovery time objectives for activities; Resource allocation and responsibilities (Business Continuity Plan E-WISE [Restricted].docx.pdf)</t>
+          <t>Business Continuity Plan E-WISE [Restricted].docx.pdf, Appendix 6 Disaster Recovery Plans (page 14); Chapter 2 Sections 2.7, 2.9, 3 (pages 7-10): 'Recovery time objectives defined'; 'Resources required listed'; 'Restoration and resumption steps described.'</t>
         </is>
       </c>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Business Continuity Plan [Confidential] referenced but not provided in evidence text.</t>
+          <t>ELEARN4_Restoring_Test_(staging).pdf</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>No direct evidence of Disaster Recovery Plans or ICT readiness details found in provided evidence text.</t>
+          <t>Restore tests for IT infrastructure (EFS and Aurora) performed successfully with documented procedures.</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Provide documented Disaster Recovery Plans and ICT readiness evidence.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
@@ -1912,12 +1912,12 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Legal, statutory, regulatory and contractual requirements are identified and referenced; GDPR compliance ensured; processing agreements signed with customers and vendors; data protection discussed regularly.</t>
+          <t>List of legal, regulatory, contractual and other requirements maintained; compliance with GDPR and other laws ensured; regular reviews and updates performed.</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Section 5.1.1 Data Protection - GDPR compliance; Section 3.1 Scope of policy; Section 9 Compliance &amp; Legal; Section 3.1 Business Continuity Plan references legal and contractual requirements; Appendix - 5 Personnel Security; Information Security Policy [Internal].docx</t>
+          <t>Business Continuity Plan E-WISE [Restricted].docx.pdf, Chapter 1 Reference documents (page 4): 'List of Legal, Regulatory, Contractual and Other Requirements'; Information Security Policy [Internal].docx, Section 5.1.1 Data Protection (page 23): 'We follow European laws and GDPR'; Section 3.1 Business Partnership Security (page 19): 'Contracts include data protection clauses.'</t>
         </is>
       </c>
       <c r="H26" t="inlineStr"/>
@@ -1929,7 +1929,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Legal, statutory, regulatory and contractual requirements identified and referenced; GDPR compliance ensured; processing agreements signed; GDPR meetings conducted.</t>
+          <t>Legal, regulatory, and contractual requirements including GDPR compliance are maintained and reviewed regularly.</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
@@ -1971,29 +1971,29 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Procedures ensure compliance with intellectual property rights including copyright, design rights, trade secrets; software licensing respected; inventory maintained; infringement risks acknowledged.</t>
+          <t>Procedures ensure compliance with intellectual property rights including copyright, design rights, trade secrets; software licensing respected; inventory maintained.</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Section 9.1 Intellectual Property Rights; 9.2 Software Licensing; 9.1.1 Procedures for legal restrictions; 9.2.2 IT-Department maintains software inventory; Information Security Policy [Internal].docx</t>
+          <t>Information Security Policy [Internal].docx, Section 9.1 Intellectual Property Rights (page 48): 'Appropriate procedures to ensure compliance with legal restrictions on intellectual property'; Section 9.2 Software Licensing: 'Employees must respect licensing agreements.'</t>
         </is>
       </c>
       <c r="H27" t="inlineStr"/>
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>No explicit evidence found in provided documents.</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>No explicit procedures or evidence related to intellectual property rights compliance found.</t>
+          <t>No documented procedures or inventory related to intellectual property rights compliance found.</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Document intellectual property rights procedures and evidence.</t>
+          <t>Develop and document procedures ensuring compliance with intellectual property rights.</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
@@ -2030,12 +2030,12 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Records and information disposal done securely; personnel information shredded or overwritten per EU law; backup and restoration policies ensure data integrity and availability.</t>
+          <t>Information disposal must be secure; personnel information shredded or overwritten per law; media disposal controlled and documented.</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Section 9.3 Information Disposal; 6.8 Backup &amp; Restoration Policy; 6.8.8 Media Disposal; 5.1.1 Data Protection; Information Security Policy [Internal].docx</t>
+          <t>Information Security Policy [Internal].docx, Section 9.3 Information Disposal (page 48): 'Information disposal must be done through secure means'; 'Personnel information must be shredded or irretrievably overwritten'; Section 6.8 Backup &amp; Restoration Policy (pages 43-46): 'Backup media stored securely and disposed with authorisation.'</t>
         </is>
       </c>
       <c r="H28" t="inlineStr"/>
@@ -2047,7 +2047,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Secure storage of decommissioned equipment; physical destruction of storage media prior to disposal; authorized disposal by specialized companies; IT staff responsible for secure handling.</t>
+          <t>Secure disposal procedures for information and media disposal are defined, including physical destruction of storage media and controlled removal by recycling companies.</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
@@ -2089,12 +2089,12 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Privacy and protection of PII ensured per relevant legislation; GDPR compliance; data incidents discussed biannually; data leaks process in place; access controls and encryption applied.</t>
+          <t>Privacy and protection of PII ensured per relevant legislation; GDPR compliance maintained; data leakage incident response defined; training and reporting in place.</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Section 3.3 Privacy and protection of PII; 5.1.1 Data Protection and GDPR compliance; 5.1.2 Data incidents and GDPR improvements; 6.10 End-point Security Policy; Information Security Policy [Internal].docx</t>
+          <t>Information Security Policy [Internal].docx, Section 5.1.1 Data Protection (page 23): 'We follow GDPR'; Section 5.1.2 Data incidents and GDPR laws discussed biannually; Business Continuity Plan E-WISE [Restricted].docx.pdf, Appendix 1 Incident Response Plan (page 11): 'Data leakage (GDPR) incident response defined.'</t>
         </is>
       </c>
       <c r="H29" t="inlineStr"/>
@@ -2106,7 +2106,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>GDPR compliance discussed; data incidents reviewed; access controls and encryption applied; data leaks process in place.</t>
+          <t>GDPR meetings conducted; data leakage incident response and training are in place; privacy and protection of PII ensured.</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
@@ -2148,12 +2148,12 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Yearly ISO internal and external audits required for all group companies; ISSC and ISWG review security policies and incidents annually; management reviews include security organisation and changes.</t>
+          <t>Annual internal and external ISO 27001 audits performed; ISSC and ISWG review security organisation and incidents; management reviews conducted yearly.</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Section 8.2.7 Yearly ISO internal and external audit; Chapter 10 Section 10.1 Review of information security; 2.1.2 and 2.1.3 Security organisation reviewed yearly by ISSC and ISWG; Information Security Policy [Internal].docx</t>
+          <t>Information Security Policy [Internal].docx, Section 8.2 Application development PEN-test &amp; audits (page 50): 'Yearly ISO internal and external audit required'; Section 2.1 Security Organisation (page 18): 'ISSC reviews yearly'; Section 10.1 Review of information security (page 37): 'Security policy reviewed yearly by ISSC and ISWG.'</t>
         </is>
       </c>
       <c r="H30" t="inlineStr"/>
@@ -2165,7 +2165,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Yearly ISO internal and external audits performed; ISSC and ISWG review security policies and incidents annually; management reviews include security organization and changes.</t>
+          <t>Annual internal and external audits performed; ISSC and ISWG review security organization and incidents; management reviews conducted yearly.</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
@@ -2207,12 +2207,12 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Compliance expected from all employees and contractors; disciplinary actions for non-compliance; policies enforced by management; audits and reviews conducted; documented procedures maintained.</t>
+          <t>Policies and standards defined and enforced; disciplinary processes for non-compliance; regular training and awareness; incident reporting and management; management reviews.</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Confidentiality Statement; Section 1.5 Roles and Responsibilities; Section 2.3 Disciplinary process; Section 9.4 Non-Compliance; Chapter 10 Evaluation and Improvement; 6.1 Documented Operating procedures; Information Security Policy [Internal].docx</t>
+          <t>Information Security Policy [Internal].docx, Section 1.5 Roles and Responsibilities (page 14); Section 2.3 Disciplinary process (page 22); Section 2.2 Information security awareness, education and training (page 22); Section 6.5 Security incident management (pages 34-36); Section 9.4 Non-Compliance (page 48); Section 10.1 Review of information security (page 37).</t>
         </is>
       </c>
       <c r="H31" t="inlineStr"/>
@@ -2224,7 +2224,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Compliance expected from all employees and contractors; disciplinary actions for non-compliance discussed; policies enforced by management; audits and reviews conducted.</t>
+          <t>Policies and standards are defined and enforced; disciplinary processes, training, incident reporting, and management reviews are documented.</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
@@ -2262,24 +2262,24 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Operating procedures are documented and maintained; changes authorized by management; procedures cover incident management, change management, backup, recovery, and system operations.</t>
+          <t>Operating procedures documented and maintained for incident management, change management, backup, recovery, system restart, and other key processes.</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Section 6.1 Documented Operating procedures; Commentary on formal documents and change authorization; Information Security Policy [Internal].docx</t>
+          <t>Information Security Policy [Internal].docx, Section 6.1 Documented Operating procedures (page 32): 'Operating procedures identified by the security policy should be documented and maintained'; 'Includes incident management, change management, backup and restoration procedures.'</t>
         </is>
       </c>
       <c r="H32" t="inlineStr"/>
       <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Reducate - Disposal of devices [Confidential].docx</t>
+          <t>Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Documented procedures for equipment disposal and handling; changes authorized by management; procedures cover incident management and change management.</t>
+          <t>Operating procedures for incident management, change management, backup, recovery, and system restart are documented and maintained.</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
@@ -2321,12 +2321,12 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Management responsibilities include setting security objectives, resource allocation, policy enforcement, training, review, and continuous improvement. Documented procedures for incident management, change management, and review processes are in place.</t>
+          <t>Management is responsible for setting security objectives, resource allocation, policy enforcement, training, review, and continuous improvement.</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Information Security Policy [Internal].docx - Section 1.5 Roles and Responsibilities; Chapter 6 IT Operations Controls; Chapter 9 Management of Information Security Incidents; Chapter 10 Evaluation and Improvement</t>
+          <t>Information Security Policy [Internal].docx: 'Section - 1.5 Roles and Responsibilities' and 'Executive responsibilities' listing management duties including setting objectives, resource management, training, review, and continuous security.</t>
         </is>
       </c>
       <c r="H33" t="inlineStr"/>
@@ -2338,7 +2338,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Management review includes setting security objectives, resource allocation, policy enforcement, training updates, review of audit results, incident management, and continual improvement actions.</t>
+          <t>Management review meetings cover setting security objectives, resource allocation, policy enforcement, training updates, audit results, and continual improvement actions.</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
@@ -2376,34 +2376,34 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Procedures exist for contacting authorities in case of incidents such as data leakage, facility disasters, and other emergencies.</t>
+          <t>Contact details and procedures for engaging with authorities in case of incidents are defined in the Business Continuity Plan and Incident Response Plan.</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Business Continuity Plan E-WISE [Restricted].docx.pdf - Appendix 1 Incident Response Plan - Facilities and infrastructure section; Contact details for authorities and insurance companies</t>
+          <t>Business Continuity Plan E-WISE [Restricted].docx.pdf: Appendix 1 Incident Response Plan (Page 11) lists contacts for local authorities, police, fire department (call 112) for facility disasters.</t>
         </is>
       </c>
       <c r="H34" t="inlineStr"/>
       <c r="I34" t="inlineStr"/>
       <c r="J34" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>No explicit procedures or references to contact with authorities in case of incidents found in the evidence text.</t>
+          <t>Business Continuity Plan and Incident Response Plan are referenced as confidential documents relevant to incident management and contact with authorities.</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Include documented procedures or evidence of contact with authorities for incidents such as data leakage or disasters.</t>
+          <t>Provide explicit procedures or contact details for authorities within the evidence.</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>🟡</t>
         </is>
       </c>
     </row>
@@ -2431,34 +2431,34 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>The document states that Reducate and group companies should regularly get security news from external vendors, forums, newsletters, or magazines to stay updated.</t>
+          <t>The organisation maintains subscriptions and receives security news from external vendors, forums, newsletters, and government security authorities.</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Information Security Policy [Internal].docx - Section 2.1 Security Organisation - 2.1.7</t>
+          <t>Information Security Policy [Internal].docx: '2.1.7 Any company part of the Reducate group should regularly get security news from external vendors, forums, newsletters or magazines...'; '2.1.8 Any company part of the Reducate group should be informed, if applicable, by local government security authorities...'</t>
         </is>
       </c>
       <c r="H35" t="inlineStr"/>
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>No mention of contact with special interest groups or regular receipt of security news from external vendors or forums.</t>
+          <t>Subscriptions and communication with external parties such as GDPR meetings and vendor risk assessments are mentioned.</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Document and provide evidence of engagement with special interest groups or receipt of security news.</t>
+          <t>Include specific examples or lists of special interest groups and subscription details.</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>🟡</t>
         </is>
       </c>
     </row>
@@ -2490,12 +2490,12 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Subscriptions to vulnerability and virus breakout notifications are maintained and circulated to relevant teams. Security news is regularly obtained from external sources.</t>
+          <t>Processes to acquire and circulate information about vulnerabilities and threats are established.</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Information Security Policy [Internal].docx - Section 2.1 Security Organisation - 2.1.7; Chapter 6 IT Operations Controls - 6.5 Security incident management</t>
+          <t>Information Security Policy [Internal].docx: '6.5 Security incident management' and '6.2 Management of technical vulnerabilities' describe acquiring vulnerability info, circulating to support teams, and maintaining subscriptions to vulnerability notifications.</t>
         </is>
       </c>
       <c r="H36" t="inlineStr"/>
@@ -2507,17 +2507,17 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>IT Security function maintains subscriptions to vulnerability notifications; monthly ISSC incident briefings include vulnerability discussions.</t>
+          <t>Risk assessments and improvements are discussed regularly, indicating processes to acquire and circulate threat intelligence.</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Document formal threat intelligence processes and circulation methods.</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>🟡</t>
         </is>
       </c>
     </row>
@@ -2549,12 +2549,12 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Information Security Steering Committee (ISSC) and Information Security Working Group (ISWG) review project plans for compliance with security policy. SDLC policies and quality checks are documented and reviewed periodically.</t>
+          <t>Security requirements are integrated into project management and system development lifecycle (SDLC) with documented policies and quality checks.</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Information Security Policy [Internal].docx - Section 2.1 Security Organisation - 2.2, 2.3; Chapter 8 Systems Development Policy - 8.1 Security in application development</t>
+          <t>Information Security Policy [Internal].docx: '8.1 Security in application development' details SDLC policies, quality checks, testing, change control, and security embedded in projects.</t>
         </is>
       </c>
       <c r="H37" t="inlineStr"/>
@@ -2566,17 +2566,17 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>Information Security Steering Committee (ISSC) and ISWG review security improvements and project compliance as part of management review and audit results.</t>
+          <t>Project management roles are included in meeting attendees; however, no explicit mention of integration of information security in project management or SDLC.</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Provide documented policies or evidence of security integration in project management and SDLC.</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>❌</t>
         </is>
       </c>
     </row>
@@ -2604,34 +2604,34 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>IT Asset Managers are responsible for maintaining an updated inventory of information assets, including classification and management.</t>
+          <t>IT Asset Managers maintain and periodically update inventories of hardware, software, and information assets with physical location and user assignment.</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Information Security Policy [Internal].docx - Section 1.5 Roles and Responsibilities; Chapter 6 IT Operations Controls - 6.11 Asset Management</t>
+          <t>Information Security Policy [Internal].docx: '6.11 Asset Management' - 'IT Asset Manager must maintain and periodically update information on the company’s hardware asset and its installed software/components, physical location, and the user assigned to the equipment.'</t>
         </is>
       </c>
       <c r="H38" t="inlineStr"/>
       <c r="I38" t="inlineStr"/>
       <c r="J38" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>Matrix rechten Zoho (Internal).pdf</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>No explicit inventory of information and associated assets or responsibility assignment found in evidence text.</t>
+          <t>IT Asset Managers maintain access rights and roles within Zoho CRM and other systems, indicating control over asset inventories and user assignments.</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Provide documented evidence of asset inventory maintenance and classification.</t>
+          <t>Include explicit inventory lists and update schedules for hardware, software, and information assets.</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>🟡</t>
         </is>
       </c>
     </row>
@@ -2663,12 +2663,12 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Background verification and competence checks performed on all candidates; includes CV checks, interviews, security tests, references, and certificates of conduct as applicable; compliant with laws and proportional to business needs.</t>
+          <t>Background verification and competence checks performed on all candidates; minimum qualifications defined; security tests for developers; documented screening process.</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Section 2.1 Screening; Background checks (Curriculum Vitae); 2 Physical/online meetings; security test via Testdome.com; former work reference; certificate of conduct (VOG); Information Security Policy [Internal].docx</t>
+          <t>Information Security Policy [Internal].docx, Chapter 2 Human Resource Security, Section 2.1 Screening (page 21): 'Background checks (CV), physical/online meetings, security test for developers, possible certificate of conduct.'</t>
         </is>
       </c>
       <c r="H39" t="inlineStr"/>
@@ -2680,17 +2680,17 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Onboarding checklist includes background verification steps such as CV checks, interviews, and security tests; documented onboarding process.</t>
+          <t>Onboarding checklist includes background verification steps and competence checks for new hires.</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Provide documented screening process and records of background checks.</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>🟡</t>
         </is>
       </c>
     </row>
@@ -2717,21 +2717,29 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>🟡</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Background verification and competence checks on candidates; documented procedures for equipment usage and return; formal termination and change of employment processes.</t>
+          <t>Section 2.1 Screening describes background checks and competence verification for candidates. Termination and change of employment processes are documented in Section 2.4 and 2.5. Employee responsibilities and compliance expectations are outlined in the Information Security Policy.</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Chapter 2 Human Resource Security, Section 2.1 Screening; Section 2.1.2 Equipment usage; Section 2.4 Termination of employment; Section 2.5 Change of employment. (Information Security Policy [Internal].docx)</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr"/>
-      <c r="I40" t="inlineStr"/>
+          <t>Information Security Policy [Internal].docx - Chapter 2 Human Resource Security, Section 2.1 Screening; Section 2.4 Termination of employment; Section 2.5 Change of employment.</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>No explicit mention of formal terms and conditions of employment including security requirements embedded in contracts or employment agreements.</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>Include explicit documented terms and conditions of employment that incorporate information security responsibilities and obligations.</t>
+        </is>
+      </c>
       <c r="J40" t="inlineStr">
         <is>
           <t>2.4.7 Template checklist indienst.PNG.pdf and 2.4.8 Template checklist uitdienst.PNG.pdf</t>
@@ -2739,7 +2747,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>Onboarding and offboarding checklists include equipment usage and return, formal termination and change of employment processes.</t>
+          <t>Screening and termination processes are documented in onboarding and offboarding checklists; employee responsibilities outlined in Information Security Policy.</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -2786,7 +2794,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Section 2.2 Information security awareness, education and training (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx - Chapter 2 Human Resource Security, Section 2.2 Information security awareness, education and training.</t>
         </is>
       </c>
       <c r="H41" t="inlineStr"/>
@@ -2798,7 +2806,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>Security training updated with new topics; training completion at 100%; communication sent to all staff; training planned for 2025.</t>
+          <t>Security training updates and awareness programs are planned and tracked with 100% completion reported.</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
@@ -2840,12 +2848,12 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Failure to comply with the Information Security Policy or related rules may result in disciplinary action including termination.</t>
+          <t>Failure to comply with the Information Security Policy or related rules may result in disciplinary action including termination of employment.</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Section 2.3 Disciplinary process; Section 9.4 Non-Compliance (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx - Chapter 2 Human Resource Security, Section 2.3 Disciplinary process.</t>
         </is>
       </c>
       <c r="H42" t="inlineStr"/>
@@ -2857,7 +2865,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Disciplinary actions for failure to comply with Information Security Policy discussed; termination included as possible action.</t>
+          <t>Disciplinary processes for non-compliance including termination are documented and enforced.</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -2899,12 +2907,12 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Access to information systems and physical access removed on termination day; return of company belongings; documented termination and role change processes.</t>
+          <t>Access to information systems and physical access are removed on the last day of employment. Company belongings must be returned. Documented termination and role change processes are in place.</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Section 2.4 Termination of employment; Section 2.5 Change of employment (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx - Chapter 2 Human Resource Security, Section 2.4 Termination of employment; Section 2.5 Change of employment.</t>
         </is>
       </c>
       <c r="H43" t="inlineStr"/>
@@ -2916,7 +2924,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Checklist includes removal of access and return of company belongings on termination day; documented termination and role change processes.</t>
+          <t>Checklist includes removal of access and return of company belongings on last day of employment.</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
@@ -2954,34 +2962,34 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>All external service providers must sign NDAs or have equivalent confidentiality clauses; third-party NDAs for employees must be approved.</t>
+          <t>All external service providers must sign NDAs or have equivalent confidentiality clauses in contracts. Employee NDAs required by third parties must be approved and signed per policy.</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Section 3.2 Non-Disclosure Agreements (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx - Section 3.2 Non-Disclosure Agreements.</t>
         </is>
       </c>
       <c r="H44" t="inlineStr"/>
       <c r="I44" t="inlineStr"/>
       <c r="J44" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>No explicit NDAs or confidentiality agreements for external providers or employees found.</t>
+          <t>NDAs and confidentiality agreements are part of vendor risk assessments and contract management.</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Provide documented NDAs and confidentiality agreements evidence.</t>
+          <t>Provide signed NDA samples and approval records.</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>🟡</t>
         </is>
       </c>
     </row>
@@ -3004,39 +3012,47 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>🟡</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Remote access requires IT department approval; mobile device policy includes registration, physical protection, encryption, and restrictions on private equipment use; home/cloud working supported.</t>
+          <t>Remote working is implied as employees except Studio Department can work from home/cloud. Mobile device policies and remote access controls are defined.</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Section 8.1 Mobile device policy; Section 6.9 Network Security Policy (remote access controls); Business Continuity Plan (Section 2.6 Sites and transportation) (Information Security Policy [Internal].docx, Business Continuity Plan E-WISE.pdf)</t>
-        </is>
-      </c>
-      <c r="H45" t="inlineStr"/>
-      <c r="I45" t="inlineStr"/>
+          <t>Business Continuity Plan E-WISE [Restricted].docx.pdf - Section 2.6 Sites and transportation; Information Security Policy [Internal].docx - Chapter 8 Mobile Computing (Telecommuting), Section 8.1 Mobile device policy; Section 6.9 Network Security Policy.</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>No explicit comprehensive remote working policy covering security controls, user responsibilities, and technical safeguards.</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>Develop and document a formal remote working policy addressing security requirements, user responsibilities, and technical controls.</t>
+        </is>
+      </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>Business Continuity Plan referenced in Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>No explicit remote working or mobile device policies found in evidence text.</t>
+          <t>Remote working allowed for most employees except Studio Department; mobile device policies and remote access controls are defined.</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Document remote working and mobile device policies and evidence of enforcement.</t>
+          <t>Provide explicit remote working policy documents.</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>🟡</t>
         </is>
       </c>
     </row>
@@ -3064,12 +3080,12 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Users must report all security violations immediately to managers or ISWG; IT Security function manages incident reporting and response.</t>
+          <t>Procedures for reporting security incidents are established. Users must report suspected security breaches immediately. Incident response plans and logs are maintained.</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Section 5.1.4 IT Security; Section 6.5 Security incident management (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx - Chapter 9 Management of Information Security Incidents, Section 9.1 Responsibilities and procedures; Business Continuity Plan E-WISE [Restricted].docx.pdf - Appendix 1 Incident Response Plan; Appendix 2 Incident Log.</t>
         </is>
       </c>
       <c r="H46" t="inlineStr"/>
@@ -3081,7 +3097,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Users instructed to report all security violations immediately; IT Security function manages incident reporting and response.</t>
+          <t>Procedures for reporting security incidents are established; users must report suspected breaches immediately; incident response plans and logs maintained.</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -3123,34 +3139,34 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Physical access secured by card swipe, key locks; central alarm system with yearly code changes; secured system racks; visitor escort policy; emergency access procedures.</t>
+          <t>Physical access is controlled via card swipe systems and personal keys. Central alarm systems per floor are in place with periodic code changes.</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Section 7.6 Physical Access (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx - Section 7.6 Physical Access, 7.6.1 and 7.6.2.</t>
         </is>
       </c>
       <c r="H47" t="inlineStr"/>
       <c r="I47" t="inlineStr"/>
       <c r="J47" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>Key holders server room _ Studios (Internal).pdf</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>No explicit physical security perimeter controls such as card swipe or alarm system mentioned.</t>
+          <t>Access to studios controlled by key holders; keys are assigned and updated; physical location details provided.</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Provide documented physical security perimeter controls.</t>
+          <t>Include evidence of card swipe systems and alarm systems per floor.</t>
         </is>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>🟡</t>
         </is>
       </c>
     </row>
@@ -3178,12 +3194,12 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Secure storage and destruction of backup media; media disposal documented and authorized; use of lockable fire-resistant storage; regular inventory and disposal controls.</t>
+          <t>Storage media disposal and handling policies are defined. Media disposal must ensure data recovery is not possible. Regular checks on portable storage device usage are performed.</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Section 6.8 Backup &amp; Restoration Policy; Section 6.10 End-point Security Policy; Section 9.3 Information Disposal (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx - Section 6.10 End-point Security Policy; Section 6.8 Backup &amp; Restoration Policy; Section 9.3 Information Disposal.</t>
         </is>
       </c>
       <c r="H48" t="inlineStr"/>
@@ -3195,7 +3211,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>Secure storage and destruction of backup media; media disposal documented and authorized; use of lockable fire-resistant storage.</t>
+          <t>Storage media disposal and handling policies defined; data recovery prevention ensured; regular checks on portable storage usage performed.</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
@@ -3228,39 +3244,47 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>🟡</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Uninterruptible power supply (UPS) in place for routers and switches; facilities managed to ensure availability of utilities.</t>
+          <t>Backup power (UPS) for network devices is specified. Electricity supply contacts and responsibilities are defined in Business Continuity Plan.</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Section 6.9.36 Network Security Policy (Information Security Policy [Internal].docx); Business Continuity Plan Section 2.9 Required resources (Business Continuity Plan E-WISE.pdf)</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr"/>
-      <c r="I49" t="inlineStr"/>
+          <t>Information Security Policy [Internal].docx - Section 6.9.36; Business Continuity Plan E-WISE [Restricted].docx.pdf - Appendix 5 Key Contacts; Section 2.9 Required resources.</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>No comprehensive documented controls for utilities supporting IT infrastructure (e.g., HVAC, water, fire suppression).</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>Develop and document controls for supporting utilities to ensure availability and protection.</t>
+        </is>
+      </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>Business Continuity Plan referenced in Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>No explicit mention of UPS or supporting utilities in evidence text.</t>
+          <t>Backup power (UPS) for network devices specified; electricity supply contacts and responsibilities defined.</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Document supporting utilities and UPS availability.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
@@ -3288,29 +3312,29 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Cabling installed and secured according to local and European regulations; regular maintenance and updates of perimeter devices including cabling.</t>
+          <t>Cabling must be installed and secured according to local or European regulations.</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Section 6.9.37 Cabling security; Section 6.9.38 Network device maintenance (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx - Section 6.9.37 Cabling security.</t>
         </is>
       </c>
       <c r="H50" t="inlineStr"/>
       <c r="I50" t="inlineStr"/>
       <c r="J50" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>No explicit evidence found in provided documents.</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>No explicit cabling security or maintenance details found.</t>
+          <t>No documentation on cabling security or installation according to regulations.</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Document cabling security controls.</t>
+          <t>Develop and document cabling security procedures.</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
@@ -3343,42 +3367,42 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Section 6.9.38 mentions that devices in the network perimeter should have regular maintenance and software updates if required or recommended by the supplier.</t>
+          <t>The Business Continuity Plan (E-WISE) mentions repair and purchasing decisions for equipment post-incident (Page 9-10). The Information Security Policy (Reducate) references regular maintenance and software updates for perimeter devices and network equipment (Section 6.9.38) and physical asset management (Section 6.11).</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>6.9.38 Any devices in the perimeters of our network should have regular maintenance and software updates if this is required or recommended by the supplier. Tv’s, portable streaming devices, presenter equipment, music systems, mobile devices and anything else which is connected to our network. (Information Security Policy [Internal].docx)</t>
+          <t>Business Continuity Plan E-WISE [Restricted].docx.pdf Pages 9-10: Section 3.2 Assessment of the situation &amp; determining options and responsibilities; Information Security Policy [Internal].docx Section 6.9.38: 'Any devices in the perimeters of our network should have regular maintenance and software updates if this is required or recommended by the supplier.' Section 6.11 Asset Management.</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>No comprehensive equipment maintenance policy covering all company equipment; focus is only on network perimeter devices.</t>
+          <t>No detailed documented procedure or schedule for equipment maintenance is described. No explicit responsibility assignment or maintenance records mentioned.</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>Develop and document a formal equipment maintenance policy covering all IT and physical equipment, including schedules, responsibilities, and procedures.</t>
+          <t>Develop and document formal equipment maintenance procedures including schedules, responsibilities, and record-keeping to ensure consistent maintenance of physical and IT equipment.</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf and Reducate - Disposal of devices [Confidential].docx</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>No explicit equipment maintenance procedures found.</t>
+          <t>Regular maintenance and software updates for perimeter devices and network equipment referenced; repair and purchasing decisions post-incident documented.</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Document equipment maintenance schedules and procedures.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
@@ -3406,12 +3430,12 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Section 6.8.8 details secure destruction of information storage media ensuring data recovery is not possible, including retention of destruction evidence. Section 6.11.4 and 6.11.5 address proper purchase and disposal of hardware and software with formal approval required for disposal.</t>
+          <t>Information disposal and media disposal policies are defined, including secure destruction of media to prevent data recovery. Return of company equipment upon termination is mandated.</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>6.8.8 Media Disposal – All information storage media containing company information classified as ‘Internal’, ‘Confidential’ or ‘Restricted’, must be destroyed, ensuring data recovery is not possible. Evidence of media destruction should be retained. (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx Sections 2.4 Termination of employment; 6.8.8 Media Disposal: 'All information storage media containing company information classified as ‘Internal’, ‘Confidential’ or ‘Restricted’, must be destroyed, ensuring data recovery is not possible.' Section 6.11.5: 'Employees are not allowed to dispose of hardware and software and take business belongings offside our offices without formal approval.'</t>
         </is>
       </c>
       <c r="H52" t="inlineStr"/>
@@ -3423,7 +3447,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Secure destruction of information storage media ensuring data recovery is not possible; retention of destruction evidence; formal approval required for disposal.</t>
+          <t>Secure disposal or reuse of equipment is defined including secure destruction of media and return of company equipment upon termination.</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
@@ -3461,34 +3485,34 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Access controlled via card swipe, keys signed out and returned; visitors escorted; third-party access controlled; emergency access procedures in place.</t>
+          <t>Access to buildings and system racks is controlled and logged. Visitors and uninducted staff must be escorted. Emergency access procedures exist.</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Section 7.6 Physical Access (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx - Section 7.6 Physical Access, 7.6.3 to 7.6.10.</t>
         </is>
       </c>
       <c r="H53" t="inlineStr"/>
       <c r="I53" t="inlineStr"/>
       <c r="J53" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>Key holders server room _ Studios (Internal).pdf</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>No explicit physical entry controls or visitor escort policies found.</t>
+          <t>Access to server rooms controlled and logged; visitors must be escorted; emergency access procedures exist.</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Document physical entry controls and visitor management.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
@@ -3516,34 +3540,34 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>System racks locked; doors locked by default; higher security levels available on request; secured storage for backup media with environmental controls.</t>
+          <t>System racks and rooms are locked by default. Higher security levels can be implemented on request. Keys are signed for and returned upon personnel leaving.</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Section 7.6 Physical Access; Section 6.8 Backup &amp; Restoration Policy (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx - Section 7.6 Physical Access, 7.6.3 to 7.6.6.</t>
         </is>
       </c>
       <c r="H54" t="inlineStr"/>
       <c r="I54" t="inlineStr"/>
       <c r="J54" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>Key holders server room _ Studios (Internal).pdf</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>No explicit securing of offices, rooms, or facilities described.</t>
+          <t>System racks and rooms are locked by default; keys signed for and returned upon personnel leaving.</t>
         </is>
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Provide evidence of securing offices and facilities.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
@@ -3575,37 +3599,37 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Central alarm system per floor with yearly code changes; no explicit mention of CCTV or continuous monitoring.</t>
+          <t>Central alarm systems exist with code changes. No explicit mention of CCTV or continuous monitoring.</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Section 7.6 Physical Access (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx - Section 7.6 Physical Access, 7.6.1.</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>No explicit mention of CCTV or physical security monitoring systems beyond alarm system.</t>
+          <t>Lack of explicit physical security monitoring controls such as CCTV or intrusion detection.</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>Implement and document physical security monitoring such as CCTV or access logs to enhance perimeter security monitoring.</t>
+          <t>Implement and document physical security monitoring measures including CCTV or intrusion detection systems.</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>No explicit evidence of CCTV or continuous physical security monitoring found.</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>Central alarm system mentioned in policy but no explicit mention of CCTV or continuous monitoring in evidence text.</t>
+          <t>Central alarm systems exist with code changes; no mention of CCTV.</t>
         </is>
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Consider adding CCTV or continuous monitoring for enhanced physical security.</t>
+          <t>Consider implementing and documenting CCTV or continuous monitoring.</t>
         </is>
       </c>
       <c r="M55" t="inlineStr">
@@ -3633,29 +3657,37 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>🟡</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Use of local country regulations for protection against natural disasters, malicious attacks or accidents; backup storage rooms equipped with fire prevention and detection, temperature and humidity control.</t>
+          <t>Local country regulations for protection against natural disasters and malicious attacks are referenced. Backup power (UPS) for network devices is specified.</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Section 7.6.12 Physical Access; Section 6.8.12 Backup &amp; Restoration Policy (Information Security Policy [Internal].docx)</t>
-        </is>
-      </c>
-      <c r="H56" t="inlineStr"/>
-      <c r="I56" t="inlineStr"/>
+          <t>Information Security Policy [Internal].docx - Section 7.6.12; Section 6.9.36 Uninterruptible power supply; Section 7.6.12.</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>No detailed documented controls for environmental threats such as fire suppression, flood protection, or environmental monitoring.</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>Develop and document comprehensive physical and environmental threat protection controls.</t>
+        </is>
+      </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Reducate - Disposal of devices [Confidential].docx</t>
+          <t>Business Continuity Plan referenced in Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>Backup storage rooms equipped with fire prevention and detection, temperature and humidity control as per local regulations.</t>
+          <t>Backup power (UPS) for network devices specified; local regulations referenced for physical and environmental threats.</t>
         </is>
       </c>
       <c r="L56" t="inlineStr">
@@ -3693,34 +3725,34 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Access to secure areas limited to authorized IT personnel and approved external vendors; visitors and uninducted staff must be escorted.</t>
+          <t>Access to secure areas is restricted to authorized personnel only. Visitors must be escorted. Emergency access procedures exist.</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Section 7.6 Physical Access (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx - Section 7.6 Physical Access, 7.6.8 and 7.6.9.</t>
         </is>
       </c>
       <c r="H57" t="inlineStr"/>
       <c r="I57" t="inlineStr"/>
       <c r="J57" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>Key holders server room _ Studios (Internal).pdf</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
         <is>
-          <t>No explicit access restrictions to secure areas or escort policies found.</t>
+          <t>Access to secure areas restricted to authorized personnel; visitors escorted; emergency access procedures exist.</t>
         </is>
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Document access controls for secure areas.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="M57" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
@@ -3748,34 +3780,34 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Clear desk recommended; no personal or critical information left unattended; locked storage provided; regular internal audits conducted.</t>
+          <t>Clear desk policy is recommended. Personal belongings should be stored securely. Regular internal audits are performed.</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Section 5.2 General Security policy (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx - Section 5.2 General Security policy, 5.2.4 Clear desk is recommended.</t>
         </is>
       </c>
       <c r="H58" t="inlineStr"/>
       <c r="I58" t="inlineStr"/>
       <c r="J58" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
         <is>
-          <t>No explicit clear desk and clear screen policies or audit evidence found.</t>
+          <t>Clear desk policy is recommended; personal belongings stored securely; regular internal audits performed.</t>
         </is>
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Implement and document clear desk/screen policies.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="M58" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
@@ -3798,39 +3830,47 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>🟡</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Equipment secured in locked racks; physical protection of mobile devices and laptops emphasized; policies for borrowing and returning equipment.</t>
+          <t>Equipment usage and return policies are defined. Physical protection of devices is mentioned in mobile device policy. No detailed equipment siting controls.</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Section 2.1.2 Equipment usage; Section 7.6 Physical Access (Information Security Policy [Internal].docx)</t>
-        </is>
-      </c>
-      <c r="H59" t="inlineStr"/>
-      <c r="I59" t="inlineStr"/>
+          <t>Information Security Policy [Internal].docx - Section 2.1.2 Equipment usage; Section 8.1 Mobile device policy.</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>Lack of explicit controls on equipment siting and physical protection measures.</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>Document and implement equipment siting and protection controls to prevent damage or theft.</t>
+        </is>
+      </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Reducate - Disposal of devices [Confidential].docx</t>
+          <t>Mobile device policy referenced in Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
         <is>
-          <t>Equipment secured in locked racks; policies for borrowing and returning equipment documented.</t>
+          <t>Physical protection of devices mentioned; no detailed equipment siting controls found.</t>
         </is>
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Develop and document equipment siting and protection controls.</t>
         </is>
       </c>
       <c r="M59" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>🟡</t>
         </is>
       </c>
     </row>
@@ -3853,39 +3893,47 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>🟡</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Mobile devices protected by encryption; policies for off-site use and return of company assets; strong discouragement of personal device use except approved mobile devices.</t>
+          <t>Mobile device policy addresses protection of devices off-site. Business Continuity Plan allows working from home for most employees. No detailed controls on off-premises asset security.</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Section 8.1 Mobile device policy; Section 6.10 End-point Security Policy (Information Security Policy [Internal].docx)</t>
-        </is>
-      </c>
-      <c r="H60" t="inlineStr"/>
-      <c r="I60" t="inlineStr"/>
+          <t>Information Security Policy [Internal].docx - Chapter 8 Mobile Computing; Business Continuity Plan E-WISE [Restricted].docx.pdf - Section 2.6 Sites and transportation.</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>No formal documented controls for security of assets when off-premises.</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>Establish and document controls for protecting assets used or stored off-premises.</t>
+        </is>
+      </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>Business Continuity Plan referenced in Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
         <is>
-          <t>No explicit policies for security of assets off-premises or mobile device encryption found.</t>
+          <t>Mobile device policy addresses off-site protection; working from home allowed; no detailed off-premises asset security controls found.</t>
         </is>
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>Document off-premises asset security policies.</t>
+          <t>Enhance controls and documentation for off-premises asset security.</t>
         </is>
       </c>
       <c r="M60" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>🟡</t>
         </is>
       </c>
     </row>
@@ -3917,34 +3965,34 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Section 2.1.2 Equipment usage defines documented procedures for borrowing company devices and return upon termination. Chapter 8 Mobile Computing (Telecommuting) Section 8.1 defines mobile device policy including registration, physical protection, encryption, and restrictions. Section 6.10 End-point Security Policy details software restrictions, patching, and virus protection on endpoint devices.</t>
+          <t>Policies cover management, registration, physical protection, and secure use of mobile and endpoint devices. Use of company-provided devices is mandated; BYOD is discouraged. Endpoint security including antivirus and patching is enforced.</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>2.1.2 Equipment usage; 8.1 Mobile device policy; 6.10 End-point Security Policy (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx Sections 5.1.4 IT Security; 5.1.11 Mobile equipment Usage; 6.6 Protection against malicious software; 6.10 End-point Security Policy; 2.1.2 Equipment usage.</t>
         </is>
       </c>
       <c r="H61" t="inlineStr"/>
       <c r="I61" t="inlineStr"/>
       <c r="J61" t="inlineStr">
         <is>
-          <t>2.4.7 Template checklist indienst.PNG.pdf and Kopie van BS02 E-Wise Wachtwoordbeleid [Internal].pdf</t>
+          <t>Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>Documented procedures for borrowing company devices and return upon termination; mobile device policy includes registration, physical protection, encryption, and restrictions; endpoint security includes software restrictions, patching, and virus protection.</t>
+          <t>Endpoint security in place with ManageEngine and Microsoft Defender; company-provided devices mandated; BYOD discouraged.</t>
         </is>
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Provide endpoint device management policy documents.</t>
         </is>
       </c>
       <c r="M61" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>🟡</t>
         </is>
       </c>
     </row>
@@ -3976,12 +4024,12 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Section 9.3 Information Disposal mandates secure disposal of information and shredding or irretrievable overwriting of personnel information. Section 6.8.8 Media Disposal details destruction of storage media ensuring data recovery is impossible with evidence retention.</t>
+          <t>Information disposal is performed securely with shredding or irretrievable overwriting. Media disposal is controlled and documented to prevent data recovery.</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>9.3 Information Disposal; 6.8.8 Media Disposal (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx Sections 9.3 Information Disposal; 6.8.8 Media Disposal.</t>
         </is>
       </c>
       <c r="H62" t="inlineStr"/>
@@ -3993,7 +4041,7 @@
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>Secure disposal of information and shredding or irretrievable overwriting of personnel information; destruction of storage media ensuring data recovery is impossible with evidence retention.</t>
+          <t>Information deletion performed securely with shredding and overwriting; media disposal controlled and documented.</t>
         </is>
       </c>
       <c r="L62" t="inlineStr">
@@ -4026,42 +4074,42 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>🟡</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Section 8.1.10 Testing states test environments should use limited, anonymised or pseudonymised data. Section 4.1.2 Handling Information Assets mentions general guidelines but no detailed data masking policy.</t>
+          <t>No explicit policy or procedure for data masking or anonymization in testing or production environments is described.</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>8.1.10 Test environments should only have limited data suitable to perform tests and preferable test data or anonymised data (data masking). (Information Security Policy [Internal].docx)</t>
+          <t>No mention found in provided documents.</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>No formal documented data masking policy or procedures for production data in non-production environments.</t>
+          <t>Lack of documented controls or procedures for data masking to protect sensitive data during testing or development.</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>Develop and implement a formal data masking policy and procedures for use of sensitive data in testing and development.</t>
+          <t>Develop and implement data masking policies and procedures to protect sensitive data in non-production environments.</t>
         </is>
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>No explicit evidence found in provided documents.</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
         <is>
-          <t>No detailed data masking policy found; general guidelines mentioned but no specifics.</t>
+          <t>No policy or procedure for data masking or anonymization described.</t>
         </is>
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Develop and document data masking policies.</t>
+          <t>Develop and document data masking and anonymization procedures.</t>
         </is>
       </c>
       <c r="M63" t="inlineStr">
@@ -4089,47 +4137,47 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>🟡</t>
+          <t>❌</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Section 4.1.3 Reporting Information Assets includes yearly review of files shared externally and cleanup procedures to prevent data breaches. Section 5.1.4 IT Security prohibits unauthorized file sharing and mandates reporting of security violations. No explicit DLP technology or controls described.</t>
+          <t>No explicit mention of data leakage prevention technologies or policies beyond incident response to data leakage.</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>4.1.3 Asset Owners should yearly review files shared with external parties; 5.1.4 Users prohibited from unauthorized file sharing. (Information Security Policy [Internal].docx)</t>
+          <t>Business Continuity Plan includes incident response for data leakage (Appendix 1), but no proactive DLP controls described.</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>No explicit data leakage prevention tools or technical controls described.</t>
+          <t>No proactive data leakage prevention controls or policies documented.</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>Implement and document technical data leakage prevention controls and monitoring.</t>
+          <t>Establish and document data leakage prevention controls and monitoring to prevent unauthorized data exfiltration.</t>
         </is>
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
+          <t>No explicit evidence found in provided documents.</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
         <is>
-          <t>Yearly review of files shared externally and cleanup procedures to prevent data breaches; unauthorized file sharing prohibited; reporting of security violations mandated.</t>
+          <t>No mention of data leakage prevention technologies or policies beyond incident response.</t>
         </is>
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>Consider implementing explicit DLP technologies.</t>
+          <t>Develop and document data leakage prevention controls.</t>
         </is>
       </c>
       <c r="M64" t="inlineStr">
         <is>
-          <t>🟡</t>
+          <t>❌</t>
         </is>
       </c>
     </row>
@@ -4161,24 +4209,24 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Section 6.8 Backup &amp; Restoration Policy details backup frequency, retention, secure storage, off-site backups, testing, disposal, and restoration drills with defined responsibilities and documentation.</t>
+          <t>Backup policies require periodic backups of critical systems and data, secure storage of backup media, offsite storage, periodic testing of backups, and documented restoration procedures.</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>6.8 Backup &amp; Restoration Policy (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx Sections 6.8 Backup &amp; Restoration Policy; Business Continuity Plan E-WISE [Restricted].docx.pdf Section 2.9 Required resources (Page 8).</t>
         </is>
       </c>
       <c r="H65" t="inlineStr"/>
       <c r="I65" t="inlineStr"/>
       <c r="J65" t="inlineStr">
         <is>
-          <t>Reducate - Disposal of devices [Confidential].docx and Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
+          <t>Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
         <is>
-          <t>Backup frequency, retention, secure storage, off-site backups, testing, disposal, and restoration drills documented; restore tests successfully done.</t>
+          <t>Backup policies require periodic backups, secure storage, offsite storage, testing, and restoration procedures; restore tests successfully done.</t>
         </is>
       </c>
       <c r="L65" t="inlineStr">
@@ -4220,22 +4268,22 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Section 6.15 Information security continuity requires a Business Continuity Plan. The Business Continuity Plan document defines recovery time objectives and alternative sites but lacks explicit redundancy controls for processing facilities.</t>
+          <t>Business Continuity Plan defines alternative sites and recovery time objectives for critical activities. However, explicit technical redundancy measures for IT processing facilities are not detailed.</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>6.15 Information security continuity; Business Continuity Plan E-WISE [Restricted].docx.pdf (Sections 2.7 Order of recovery for activities, 2.6 Sites and transportation)</t>
+          <t>Business Continuity Plan E-WISE [Restricted].docx.pdf Sections 2.6 Sites and transportation; 2.7 Order of recovery for activities; Appendix 3 List of Business Continuity Sites.</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>No explicit documented redundancy measures for information processing facilities.</t>
+          <t>No detailed technical redundancy controls or infrastructure redundancy plans described.</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>Document and implement redundancy controls for critical information processing facilities to ensure availability.</t>
+          <t>Document and implement technical redundancy measures for critical IT processing facilities to ensure availability.</t>
         </is>
       </c>
       <c r="J66" t="inlineStr">
@@ -4245,12 +4293,12 @@
       </c>
       <c r="K66" t="inlineStr">
         <is>
-          <t>Business Continuity Plan defines recovery time objectives and alternative sites; lacks explicit redundancy controls for processing facilities.</t>
+          <t>Business Continuity Plan defines alternative sites and recovery time objectives; no explicit technical redundancy measures detailed.</t>
         </is>
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Consider adding explicit redundancy controls for processing facilities.</t>
+          <t>Consider documenting technical redundancy measures for IT processing facilities.</t>
         </is>
       </c>
       <c r="M66" t="inlineStr">
@@ -4287,24 +4335,24 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Section 6.14 Logging and Audit Policy mandates time synchronization, logging of all access from vendors and internal users, secure storage and backup of logs, and restrictions on sensitive data in logs.</t>
+          <t>Logging policies require synchronized clocks, logging of all access, secure storage and backup of logs, and regular monitoring. Logs exclude sensitive personal data.</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>6.14 Logging and Audit Policy (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx Sections 6.14 Logging and Audit Policy.</t>
         </is>
       </c>
       <c r="H67" t="inlineStr"/>
       <c r="I67" t="inlineStr"/>
       <c r="J67" t="inlineStr">
         <is>
-          <t>Log retention (Internal).pdf and Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
+          <t>Log retention (Internal).pdf</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
         <is>
-          <t>Logging and audit policy mandates time synchronization; logging of all access from vendors and internal users; secure storage and backup of logs; restrictions on sensitive data in logs.</t>
+          <t>Logging policies require synchronized clocks, logging of access, secure storage and backup of logs; retention periods defined per system.</t>
         </is>
       </c>
       <c r="L67" t="inlineStr">
@@ -4346,12 +4394,12 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Section 9.1 Responsibilities and procedures defines management procedures for monitoring, detecting, analyzing, and reporting information security events and incidents with escalation and recovery processes.</t>
+          <t>Procedures for monitoring, detecting, analyzing, and reporting information security events are established. Incident management and response processes are documented.</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>9.1 Responsibilities and procedures (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx Section 9.1 Responsibilities and procedures; Section 6.5 Security incident management.</t>
         </is>
       </c>
       <c r="H68" t="inlineStr"/>
@@ -4363,7 +4411,7 @@
       </c>
       <c r="K68" t="inlineStr">
         <is>
-          <t>Management procedures for monitoring, detecting, analyzing, and reporting information security events and incidents with escalation and recovery processes defined.</t>
+          <t>Monitoring, detection, analysis, and reporting procedures established; incident management documented.</t>
         </is>
       </c>
       <c r="L68" t="inlineStr">
@@ -4410,19 +4458,19 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Section 6.14 Logging and Audit Policy, 6.14.1 Clock synchronisation - All computing systems managed must synchronise time with a central time server. (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx - Section 6.14 Logging and Audit Policy - 6.14.1 Clock synchronisation</t>
         </is>
       </c>
       <c r="H69" t="inlineStr"/>
       <c r="I69" t="inlineStr"/>
       <c r="J69" t="inlineStr">
         <is>
-          <t>Log retention (Internal).pdf and Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
+          <t>Log retention (Internal).pdf</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>All computing systems synchronise time with a central time server to ensure accuracy of audit logs.</t>
+          <t>All computing systems synchronize time with a central time server to ensure audit log accuracy.</t>
         </is>
       </c>
       <c r="L69" t="inlineStr">
@@ -4460,29 +4508,29 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Privileged utility programs or software should be approved by the IT department or system administrator. Laptops and desktops are pre-installed by IT with no administrator privileges enabled.</t>
+          <t>Privileged utility programs or software should be approved by the IT department or system administrator; laptops/desktops have no admin privileges enabled.</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Section 7.2.9 - A laptop or desktop computer used by employees are pre-installed by the IT department and there are no administrator privileges enabled. Privileged utility programs or software should be approved by the IT department or system administrator. (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx - Section 7.2.9 Management of privileged access rights</t>
         </is>
       </c>
       <c r="H70" t="inlineStr"/>
       <c r="I70" t="inlineStr"/>
       <c r="J70" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>No explicit evidence found in provided documents.</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>No explicit approval process for privileged utility programs or software found.</t>
+          <t>No documentation on approval or control of privileged utility programs.</t>
         </is>
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>Document approval and control of privileged utility programs.</t>
+          <t>Develop and document controls for privileged utility programs.</t>
         </is>
       </c>
       <c r="M70" t="inlineStr">
@@ -4515,34 +4563,34 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Users may not load any software not provided by Reducate’s or group companies IT-department. Only licensed software owned by Reducate or Group Companies is allowed. Unauthorized software installation is prohibited.</t>
+          <t>Users are prohibited from installing unauthorized software; only licensed software owned by the company is allowed; IT department manages software installation.</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>Section 5.1.4 IT Security - Users may not load onto computers any software not provided by Reducate’s or group companies IT-department. Section 6.10 End-point Security Policy - PCs not managed by Administrators but by IT-Department personnel are only allowed to install licensed software which are owned by Reducate or Group Companies. Illegal or inappropriate software is not allowed. (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx - Section 5.1.4 IT Security; Section 6.10 End-point Security Policy - 6.10.7</t>
         </is>
       </c>
       <c r="H71" t="inlineStr"/>
       <c r="I71" t="inlineStr"/>
       <c r="J71" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
         </is>
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>No explicit controls prohibiting unauthorized software installation found.</t>
+          <t>Users prohibited from installing unauthorized software; IT department manages software installation.</t>
         </is>
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Document software installation policies and enforcement.</t>
+          <t>Provide formal documented policy on software installation.</t>
         </is>
       </c>
       <c r="M71" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>🟡</t>
         </is>
       </c>
     </row>
@@ -4570,24 +4618,24 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Section 5.3 Management of privileged access rights describes restricted assignment of privileged access based on minimum business need, authorization processes, and separation of privileged IDs from regular user IDs. Section 7.4 User Access Management includes formal procedures for allocation and control of privileges.</t>
+          <t>Privileged access rights are restricted and controlled by formal authorization processes. Privileged accounts are separated from regular user accounts. Records of privileges are maintained.</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>5.3 Management of privileged access rights; 7.4 User Access Management (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx Section 5.3 Management of privileged access rights: 'The assignment of privileged access rights... includes assigning based on minimum requirement, maintaining authorization records, and separation from regular user IDs.'</t>
         </is>
       </c>
       <c r="H72" t="inlineStr"/>
       <c r="I72" t="inlineStr"/>
       <c r="J72" t="inlineStr">
         <is>
-          <t>Matrix rechten Zoho (Internal).pdf and Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
+          <t>Matrix rechten Zoho (Internal).pdf</t>
         </is>
       </c>
       <c r="K72" t="inlineStr">
         <is>
-          <t>Privileged access rights restricted based on minimum business need; authorization processes in place; separation of privileged IDs from regular user IDs; formal procedures for allocation and control of privileges.</t>
+          <t>Privileged access rights are controlled with formal authorization; privileged accounts separated from regular users; records maintained.</t>
         </is>
       </c>
       <c r="L72" t="inlineStr">
@@ -4629,34 +4677,34 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Network security is maintained by using firewalls, authorization, access control, monitoring logs, encryption for data over public networks, and restricting network connectivity to approved devices and users.</t>
+          <t>Network security is maintained via firewalls, access control, logging, encryption for public networks, and regular patching of network devices.</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Section 7.1 Network controls - Use of firewalls, authorization, access control, and monitoring logs. Section 6.9 Network Security Policy - All connections to external networks must be approved, firewalls must be ICSA certified, firewall rules must drop unauthorized packets, and all changes logged. (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx - Chapter 7 Security of Communication - Section 7.1 Network controls; Section 6.9 Network Security Policy</t>
         </is>
       </c>
       <c r="H73" t="inlineStr"/>
       <c r="I73" t="inlineStr"/>
       <c r="J73" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>Log retention (Internal).pdf</t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
         <is>
-          <t>No explicit network security controls such as firewalls, encryption, or access restrictions described.</t>
+          <t>Network security maintained via firewalls, access control, logging, encryption for public networks, and regular patching.</t>
         </is>
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>Document network security controls and monitoring.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="M73" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
@@ -4684,34 +4732,34 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Network services are secured by restricting access, using firewalls, logging, and ensuring only authorized connections are allowed. Remote access requires approval.</t>
+          <t>Network services are controlled with firewalls, access restrictions, logging, and encryption; remote access requires approval.</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Section 6.9 Network Security Policy - Access to LAN/WAN devices restricted by access rules or user authentication. Remote access requires IT-department approval. Firewalls restrict traffic to/from partners/vendors. (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx - Section 6.9 Network Security Policy; Section 7.1 Network controls</t>
         </is>
       </c>
       <c r="H74" t="inlineStr"/>
       <c r="I74" t="inlineStr"/>
       <c r="J74" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
         </is>
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>No explicit security controls for network services or remote access approval found.</t>
+          <t>Network services controlled with firewalls, access restrictions, logging, and encryption; remote access requires approval.</t>
         </is>
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>Document security of network services and remote access controls.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="M74" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
@@ -4739,34 +4787,34 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Company network is logically separated and firewalls are installed to prevent unauthorized access from public or wireless networks.</t>
+          <t>Logical separation of networks is enforced; firewalls installed to prevent unauthorized access from public or wireless networks.</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Section 7.2 Segregation in networks - Firewalls must be installed and the Company's network is to be logically separated. (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx - Section 7.2 Segregation in networks</t>
         </is>
       </c>
       <c r="H75" t="inlineStr"/>
       <c r="I75" t="inlineStr"/>
       <c r="J75" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
         </is>
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>No explicit segregation of networks or firewall controls described.</t>
+          <t>Logical separation of networks enforced; firewalls installed to prevent unauthorized access from public or wireless networks.</t>
         </is>
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>Document network segregation and firewall implementation.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="M75" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
@@ -4798,34 +4846,34 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Web filtering or URL filtering is implemented on firewalls, routers, or switches to block web traffic and protect against threats and enforce policies.</t>
+          <t>Web filtering or URL filtering is implemented on firewalls, routers, or switches to block web traffic and enforce policies.</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>Section 6.9.39 Web group filtering or URL Filtering should be implemented on your firewall, routers or switches to block web traffic in order to protect against potential threats and enforce corporate or legal policies and regulations. (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx - Section 6.9.39 Web group filtering or URL Filtering</t>
         </is>
       </c>
       <c r="H76" t="inlineStr"/>
       <c r="I76" t="inlineStr"/>
       <c r="J76" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
         </is>
       </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>No explicit web filtering or URL filtering controls described.</t>
+          <t>Web filtering implemented on firewalls and routers to block web traffic and enforce policies.</t>
         </is>
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>Implement and document web filtering controls.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="M76" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
@@ -4853,34 +4901,34 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Encryption is used for HDDs (Bitlocker, Filevault, Ecryptfs), VPN connections (IPSec with 3DES or AES-256), wireless networks (WPA/WPA2), and cloud applications (TLS 1.2+). Annual testing of TLS security is performed.</t>
+          <t>Encryption is used for HDDs (Bitlocker, Filevault, Ecryptfs), VPNs (IPSec with 3DES or AES-256), wireless networks (WPA/WPA2), and TLS 1.2+ for cloud applications.</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Chapter 10 Cryptography - HDD encryption for notebooks, VPN encryption standards, wireless encryption protocols, cloud applications require TLS 1.2 or higher, yearly TLS testing at SSLlabs. (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx - Chapter 10 Cryptography</t>
         </is>
       </c>
       <c r="H77" t="inlineStr"/>
       <c r="I77" t="inlineStr"/>
       <c r="J77" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
         </is>
       </c>
       <c r="K77" t="inlineStr">
         <is>
-          <t>No explicit cryptography usage details found in evidence text.</t>
+          <t>Encryption used for HDDs (Bitlocker), VPNs (IPSec with AES-256), wireless networks (WPA2), and TLS 1.2+ for cloud applications.</t>
         </is>
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>Document cryptography usage and testing.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="M77" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
@@ -4908,12 +4956,12 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Documented SDLC policies and procedures exist for in-house and outsourced development. Quality checks, contract reviews, progress reports, testing, and documentation are required. Outsourced development reviewed for licensing and IP rights.</t>
+          <t>SDLC policies and procedures are documented; external providers' SDLC reviewed; quality checks and testing performed; code reviews and secure coding guidelines enforced.</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Section 8.1 Security in application development - Documented SDLC policies, review of outsourced development, quality checks, and periodic review of SDLC methodology. (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx - Chapter 8 Systems Development Policy - Section 8.1 Security in application development</t>
         </is>
       </c>
       <c r="H78" t="inlineStr"/>
@@ -4925,7 +4973,7 @@
       </c>
       <c r="K78" t="inlineStr">
         <is>
-          <t>Documented SDLC policies and procedures exist; quality checks, contract reviews, progress reports, testing, and documentation required; outsourced development reviewed for licensing and IP rights.</t>
+          <t>SDLC policies and procedures documented; external providers' SDLC reviewed; quality checks and testing performed; code reviews enforced.</t>
         </is>
       </c>
       <c r="L78" t="inlineStr">
@@ -4967,12 +5015,12 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Security requirements are identified and agreed prior to development. Access control to source code, audit trails, and data validation are implemented. Encryption and privacy protections are incorporated in applications.</t>
+          <t>Security requirements identified and agreed prior to development; audit trails and access controls implemented; data input validated; privacy and encryption enforced.</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Section 8.1.23 - Application forms and input fields ensure authentication, secrecy, privacy, and encryption. Section 8.1.8 - Access control to program source library. (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx - Section 8.1.23 Application security requirements</t>
         </is>
       </c>
       <c r="H79" t="inlineStr"/>
@@ -4984,7 +5032,7 @@
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>Security requirements identified and agreed prior to development; access control to source code, audit trails, and data validation implemented; encryption and privacy protections incorporated.</t>
+          <t>Application security requirements identified and agreed prior to development; audit trails and access controls implemented; data input validated.</t>
         </is>
       </c>
       <c r="L79" t="inlineStr">
@@ -4999,11 +5047,7 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
+      <c r="A80" t="inlineStr"/>
       <c r="B80" t="inlineStr">
         <is>
           <t>A.8 (Technological Controls)</t>
@@ -5011,31 +5055,39 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>A.8.28</t>
+          <t>A.8.27</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Secure coding</t>
+          <t>Secure systems architecture and engineering principles</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>🟡</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Code is reviewed by skilled personnel other than the author against secure coding guidelines. Development code is stored in secure repositories with access control and versioning.</t>
+          <t>System hardening and minimal package installation for Unix systems; IP restrictions and secure communication enforced; change management applied.</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>Section 8.1.17 - Development code stored in secure repository with access control. Section 8.1.18 - Code reviewed prior to release by skilled personnel against secure coding guidelines. (Information Security Policy [Internal].docx)</t>
-        </is>
-      </c>
-      <c r="H80" t="inlineStr"/>
-      <c r="I80" t="inlineStr"/>
+          <t>Information Security Policy [Internal].docx - Section 6.12 Systems Security Policy - Unix Systems</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>No explicit mention of formal secure architecture design principles or documented architecture standards.</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>Develop and document secure systems architecture and engineering principles aligned with ISO 27001 requirements.</t>
+        </is>
+      </c>
       <c r="J80" t="inlineStr">
         <is>
           <t>Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
@@ -5043,7 +5095,7 @@
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>Code reviewed by skilled personnel other than author against secure coding guidelines; development code stored in secure repositories with access control and versioning.</t>
+          <t>System hardening and minimal package installation for Unix systems; IP restrictions and secure communication enforced; change management applied.</t>
         </is>
       </c>
       <c r="L80" t="inlineStr">
@@ -5060,7 +5112,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>6</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -5070,12 +5122,12 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>A.8.29</t>
+          <t>A.8.28</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Security testing in development and acceptance</t>
+          <t>Secure coding</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -5085,12 +5137,12 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Application security testing is performed manually and automatically before acceptance. PEN-tests are conducted annually or after significant changes. Test environments use anonymized or masked data. Test data is removed before production deployment.</t>
+          <t>Code reviews performed by personnel other than the author; secure coding guidelines followed; code stored in secure repositories with access control and versioning.</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>Section 8.1.19 - Application security testing manual and automated. Section 8.2 Application development PEN-test &amp; audits - PEN-tests yearly, controlled environment, fix timelines. Section 8.1.21 - No production data used for testing; data is sanitized or anonymized. (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx - Section 8.1.17 and 8.1.18 Secure coding and code review</t>
         </is>
       </c>
       <c r="H81" t="inlineStr"/>
@@ -5102,7 +5154,7 @@
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>Application security testing performed manually and automatically before acceptance; PEN-tests conducted annually or after significant changes; test environments use anonymized or masked data; test data removed before production deployment.</t>
+          <t>Code reviews performed by personnel other than the author; secure coding guidelines followed; code stored in secure repositories with access control and versioning.</t>
         </is>
       </c>
       <c r="L81" t="inlineStr">
@@ -5129,12 +5181,12 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>A.8.3</t>
+          <t>A.8.29</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Information access restriction</t>
+          <t>Security testing in development and acceptance</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -5144,24 +5196,24 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Section 5.2 Information access restriction mandates access control on a need-to-know basis aligned with business requirements and classification. Section 7 Access Control policy details user registration, de-registration, and access control based on business needs and security requirements.</t>
+          <t>Application security testing performed manually and automatically; PEN-tests conducted annually; acceptance criteria defined and tested; test environments separated and use anonymized data.</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>5.2 Information access restriction; 7 Access Control policy (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx - Section 8.1.19, 8.1.20, 8.2 Application testing and PEN-tests</t>
         </is>
       </c>
       <c r="H82" t="inlineStr"/>
       <c r="I82" t="inlineStr"/>
       <c r="J82" t="inlineStr">
         <is>
-          <t>Matrix rechten Zoho (Internal).pdf and Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
+          <t>Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
         </is>
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>Access control on a need-to-know basis aligned with business requirements and classification; user registration, de-registration, and access control based on business needs and security requirements.</t>
+          <t>Application security testing performed manually and automatically; PEN-tests conducted annually; acceptance criteria defined and tested; test environments separated and use anonymized data.</t>
         </is>
       </c>
       <c r="L82" t="inlineStr">
@@ -5176,7 +5228,11 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="inlineStr"/>
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
       <c r="B83" t="inlineStr">
         <is>
           <t>A.8 (Technological Controls)</t>
@@ -5184,12 +5240,12 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>A.8.30</t>
+          <t>A.8.3</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Outsourced development</t>
+          <t>Information access restriction</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -5199,24 +5255,24 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Outsourced development requires review of SDLC methodology, licensing, code ownership, and intellectual property rights agreed in contracts. ISO certifications and PEN-tests are required for outsourced contractors.</t>
+          <t>Access to information and systems is controlled on a need-to-know basis aligned with business requirements and classification. Formal user registration and de-registration processes exist.</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Section 8.1.1 - Review of outsourced SDLC. Section 8.1.2 - Licensing and IP rights agreed before project start. Section 8.2.5 - Outsourced contractors require ISO certifications and PEN-tests. (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx Section 5.2 Information access restriction; Section 7.4 User Access Management; Section 5.2.1 Access Control policy.</t>
         </is>
       </c>
       <c r="H83" t="inlineStr"/>
       <c r="I83" t="inlineStr"/>
       <c r="J83" t="inlineStr">
         <is>
-          <t>Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
+          <t>Matrix rechten Zoho (Internal).pdf</t>
         </is>
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>Outsourced development requires review of SDLC methodology, licensing, code ownership, and IP rights agreed in contracts; ISO certifications and PEN-tests required for outsourced contractors.</t>
+          <t>Access to information and systems controlled on need-to-know basis; formal user registration and de-registration processes exist.</t>
         </is>
       </c>
       <c r="L83" t="inlineStr">
@@ -5231,11 +5287,7 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
+      <c r="A84" t="inlineStr"/>
       <c r="B84" t="inlineStr">
         <is>
           <t>A.8 (Technological Controls)</t>
@@ -5243,12 +5295,12 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>A.8.31</t>
+          <t>A.8.30</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Separation of development, test and production environments</t>
+          <t>Outsourced development</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -5258,12 +5310,12 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Development, test, and production environments are separated and do not share components. Test environments use limited or anonymized data. Migration to production requires approval and follows change control.</t>
+          <t>Outsourced development requires contract agreements covering licensing, code ownership, and security; external providers' SDLC reviewed; security requirements included in contracts.</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>Section 8.1.15 - Separation of environments. Section 8.1.10 - Test environments use limited/anonymized data. Section 8.1.22 - Code promoted to production by approved personnel following change control. (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx - Section 8.1.1, 8.1.2, 3.1 Business partnership and Outsourcing</t>
         </is>
       </c>
       <c r="H84" t="inlineStr"/>
@@ -5275,7 +5327,7 @@
       </c>
       <c r="K84" t="inlineStr">
         <is>
-          <t>Development, test, and production environments separated; test environments use limited or anonymized data; migration to production requires approval and follows change control.</t>
+          <t>Outsourced development requires contract agreements covering licensing, code ownership, and security; external providers' SDLC reviewed; security requirements included in contracts.</t>
         </is>
       </c>
       <c r="L84" t="inlineStr">
@@ -5292,7 +5344,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>6</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -5302,12 +5354,12 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>A.8.32</t>
+          <t>A.8.31</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Change management</t>
+          <t>Separation of development, test and production environments</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -5317,12 +5369,12 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Change management is documented with strict review, approval, and closure controls. All changes including emergency changes are documented and follow formal processes. Change management is integrated with development and operational procedures.</t>
+          <t>Development, test, and production environments are separated with restricted access; test data is anonymized; no development files or test data in production.</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>Section 6.2 Operational change control - Documented change management with review and approval. Section 8.1.11-8.1.13 - Program changes standardized, documented, approved, and controlled. (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx - Section 8.1.14, 8.1.15, 8.1.21, 8.1.22</t>
         </is>
       </c>
       <c r="H85" t="inlineStr"/>
@@ -5334,7 +5386,7 @@
       </c>
       <c r="K85" t="inlineStr">
         <is>
-          <t>Change management documented with strict review, approval, and closure controls; all changes including emergency changes documented and follow formal processes; integrated with development and operational procedures.</t>
+          <t>Development, test, and production environments separated with restricted access; test data anonymized; no development files or test data in production.</t>
         </is>
       </c>
       <c r="L85" t="inlineStr">
@@ -5349,7 +5401,11 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="inlineStr"/>
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
       <c r="B86" t="inlineStr">
         <is>
           <t>A.8 (Technological Controls)</t>
@@ -5357,12 +5413,12 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>A.8.33</t>
+          <t>A.8.32</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Test information</t>
+          <t>Change management</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -5372,12 +5428,12 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Test environments use limited or anonymized data. Unused test environments or sandboxes are reviewed and removed biannually. Test data is removed before production deployment.</t>
+          <t>Formal change management process with review, approval, testing, and communication; all changes documented including emergency changes; configuration management maintained.</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Section 8.1.10 - Test environments use limited/anonymized data. Unused test environments checked and removed half-yearly. Section 8.1.22 - Test data removed before production. (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx - Section 6.2 Operational change control; Section 6.3 Configuration Management; Section 8.1.11, 8.1.12, 8.1.13</t>
         </is>
       </c>
       <c r="H86" t="inlineStr"/>
@@ -5389,7 +5445,7 @@
       </c>
       <c r="K86" t="inlineStr">
         <is>
-          <t>Test environments use limited or anonymized data; unused test environments or sandboxes reviewed and removed biannually; test data removed before production deployment.</t>
+          <t>Formal change management process with review, approval, testing, and communication; all changes documented including emergency changes; configuration management maintained.</t>
         </is>
       </c>
       <c r="L86" t="inlineStr">
@@ -5412,57 +5468,49 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>A.8.34</t>
+          <t>A.8.33</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Protection of information systems during audit testing</t>
+          <t>Test information</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>🟡</t>
+          <t>✅</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Annual ISO internal and external audits are required for each group company. PEN-tests are performed in controlled environments. However, explicit controls for protecting systems during audit testing are not detailed.</t>
+          <t>Test environments use limited, anonymized or pseudonymized data; production data is not used for testing; unused test environments reviewed and removed periodically.</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>Section 8.2.7 - Yearly ISO internal and external audit required. Section 8.2.2 - PEN-tests only in controlled testing environment. (Information Security Policy [Internal].docx)</t>
-        </is>
-      </c>
-      <c r="H87" t="inlineStr">
-        <is>
-          <t>No explicit documented procedures or controls for protecting information systems during audit testing are described.</t>
-        </is>
-      </c>
-      <c r="I87" t="inlineStr">
-        <is>
-          <t>Develop and document specific procedures to protect information systems during audit and penetration testing, including scope, authorization, and impact mitigation.</t>
-        </is>
-      </c>
+          <t>Information Security Policy [Internal].docx - Section 8.1.10, 8.1.21</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr"/>
+      <c r="I87" t="inlineStr"/>
       <c r="J87" t="inlineStr">
         <is>
-          <t>Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
+          <t>No explicit evidence found in provided documents.</t>
         </is>
       </c>
       <c r="K87" t="inlineStr">
         <is>
-          <t>Annual ISO internal and external audits required; PEN-tests performed in controlled environments; no explicit controls for protecting systems during audit testing detailed.</t>
+          <t>No documented policy on test information using anonymized or pseudonymized data.</t>
         </is>
       </c>
       <c r="L87" t="inlineStr">
         <is>
-          <t>Develop explicit controls for protecting information systems during audit testing.</t>
+          <t>Develop and document test information handling procedures.</t>
         </is>
       </c>
       <c r="M87" t="inlineStr">
         <is>
-          <t>🟡</t>
+          <t>❌</t>
         </is>
       </c>
     </row>
@@ -5475,44 +5523,52 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>A.8.4</t>
+          <t>A.8.34</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Access to source code</t>
+          <t>Protection of information systems during audit testing</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>🟡</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Section 8.1.8 states access control should be implemented to restrict access to the program source library. Section 8.1.17 states development code is stored in a secure repository enforcing access control and segregation of duties.</t>
+          <t>Security incident management and logging policies exist; no explicit mention of controls specifically protecting systems during audit testing.</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>8.1.8 Access control should be implemented to restrict access to the program source library; 8.1.17 Development code is stored in a secure code repository that enforces and meets the requirements of the access control policy and segregation of duty. (Information Security Policy [Internal].docx)</t>
-        </is>
-      </c>
-      <c r="H88" t="inlineStr"/>
-      <c r="I88" t="inlineStr"/>
+          <t>Information Security Policy [Internal].docx - Section 6.5 Security incident management; Section 6.14 Logging and Audit Policy</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>No explicit documented controls or procedures to protect information systems specifically during audit testing.</t>
+        </is>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>Develop and document procedures to protect information systems during audit testing to prevent disruption or unauthorized access.</t>
+        </is>
+      </c>
       <c r="J88" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>No explicit evidence found in provided documents.</t>
         </is>
       </c>
       <c r="K88" t="inlineStr">
         <is>
-          <t>No explicit access control to source code or secure repository evidence found.</t>
+          <t>No specific controls protecting information systems during audit testing described.</t>
         </is>
       </c>
       <c r="L88" t="inlineStr">
         <is>
-          <t>Document access controls for source code repositories.</t>
+          <t>Develop and document controls for protection during audit testing.</t>
         </is>
       </c>
       <c r="M88" t="inlineStr">
@@ -5530,12 +5586,12 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>A.8.5</t>
+          <t>A.8.4</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Secure authentication</t>
+          <t>Access to source code</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
@@ -5545,91 +5601,79 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Section 4.1 Use of secret authentication information outlines password confidentiality, avoidance of insecure storage, and quality password selection. Section 7.2 Authorisation and Access Control mandates two-factor authentication and session management. Section 7.3 Password Policy details password complexity, change requirements, and secure handling.</t>
+          <t>Access to program source libraries is restricted. Development code is stored in secure repositories enforcing access control and segregation of duties. Code reviews are performed by personnel other than the author.</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>4.1 Use of secret authentication information; 7.2 Authorisation and Access Control; 7.3 Password Policy (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx Sections 8.1.8 Access control to source code; 8.1.17 Development code repository; 8.1.18 Code review.</t>
         </is>
       </c>
       <c r="H89" t="inlineStr"/>
       <c r="I89" t="inlineStr"/>
       <c r="J89" t="inlineStr">
         <is>
+          <t>No explicit evidence found in provided documents.</t>
+        </is>
+      </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>No documentation on access control to source code or secure repositories.</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>Develop and document access controls and segregation of duties for source code.</t>
+        </is>
+      </c>
+      <c r="M89" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr"/>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>A.8 (Technological Controls)</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>A.8.5</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Secure authentication</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Strong password policies are enforced including minimum length, complexity, and change requirements. Two-factor authentication is mandated where possible. Passwords must be kept confidential and not shared or stored insecurely.</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Information Security Policy [Internal].docx Sections 4.1 Use of secret authentication information; 7.3 Password Policy; 7.2.2 Two-factor authentication.</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr"/>
+      <c r="I90" t="inlineStr"/>
+      <c r="J90" t="inlineStr">
+        <is>
           <t>Kopie van BS02 E-Wise Wachtwoordbeleid [Internal].pdf</t>
         </is>
       </c>
-      <c r="K89" t="inlineStr">
-        <is>
-          <t>Password confidentiality, complexity, change requirements, and secure handling defined; two-factor authentication enforced; session management policies in place.</t>
-        </is>
-      </c>
-      <c r="L89" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="M89" t="inlineStr">
-        <is>
-          <t>✅</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>A.8 (Technological Controls)</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>A.8.6</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>Capacity management</t>
-        </is>
-      </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>✅</t>
-        </is>
-      </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>Section 3.3.1 Business Partnership Contracts includes capacity utilisation monitoring and planning as a contract area. Section 6.13.13 Database Security Policy mentions monitoring system and audit logs for capacity thresholds. Section 6.8 Backup &amp; Restoration Policy includes monitoring disk space utilisation.</t>
-        </is>
-      </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>3.3.1 Business Partnership Contracts; 6.13.13 System and audit logs are to be monitored regularly to alert of any capacity thresholds being crossed; 6.7.5 Disk space utilisation must be periodically or continuously monitored. (Information Security Policy [Internal].docx)</t>
-        </is>
-      </c>
-      <c r="H90" t="inlineStr">
-        <is>
-          <t>No explicit documented capacity management process or formal capacity planning policy.</t>
-        </is>
-      </c>
-      <c r="I90" t="inlineStr">
-        <is>
-          <t>Develop and document a formal capacity management process including monitoring, forecasting, and resource planning.</t>
-        </is>
-      </c>
-      <c r="J90" t="inlineStr">
-        <is>
-          <t>Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
-        </is>
-      </c>
       <c r="K90" t="inlineStr">
         <is>
-          <t>Capacity utilization monitoring and planning included in business partnership contracts; monitoring system and audit logs for capacity thresholds; disk space utilization monitored.</t>
+          <t>Strong password policies enforced including length, complexity, history, expiration, and two-factor authentication.</t>
         </is>
       </c>
       <c r="L90" t="inlineStr">
@@ -5656,12 +5700,12 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>A.8.7</t>
+          <t>A.8.6</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Protection against malware</t>
+          <t>Capacity management</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
@@ -5671,34 +5715,34 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Section 6.1 Controls against malware defines prevention, detection, and recovery measures including anti-virus software installation and updates, blocking unauthorized software, and proxy filtering. Section 6.6 Protection against malicious software details antivirus requirements, real-time scanning, virus handling, and update logging.</t>
+          <t>Capacity utilisation monitoring and planning is included in business partnership contracts and change management. Network and system capacity are monitored and managed.</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>6.1 Controls against malware; 6.6 Protection against malicious software (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx Section 3.3 Business Partnership Contracts; Section 6.9 Network Security Policy; Section 6.1 Documented Operating procedures.</t>
         </is>
       </c>
       <c r="H91" t="inlineStr"/>
       <c r="I91" t="inlineStr"/>
       <c r="J91" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
         </is>
       </c>
       <c r="K91" t="inlineStr">
         <is>
-          <t>No explicit malware protection policies or antivirus details found.</t>
+          <t>Capacity utilization monitoring and planning included in business partnership contracts and change management.</t>
         </is>
       </c>
       <c r="L91" t="inlineStr">
         <is>
-          <t>Document malware protection controls and evidence of implementation.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="M91" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
@@ -5715,12 +5759,12 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>A.8.8</t>
+          <t>A.8.7</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Management of technical vulnerabilities</t>
+          <t>Protection against malware</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
@@ -5730,12 +5774,12 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Section 6.2 Management of technical vulnerabilities describes processes for acquiring vulnerability information, identification, evaluation, testing, and deployment of patches. Section 8.2 Application development PEN-test &amp; audits includes PEN-testing and vulnerability remediation timelines.</t>
+          <t>Anti-malware controls include prohibition of unauthorized software, mandatory antivirus installation and updates, real-time scanning, and incident reporting procedures.</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>6.2 Management of technical vulnerabilities; 8.2 Application development PEN-test &amp; audits (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx Sections 6.6 Protection against malicious software; 5.1.4 IT Security; Appendix 6.6 Protection against malicious software.</t>
         </is>
       </c>
       <c r="H92" t="inlineStr"/>
@@ -5747,7 +5791,7 @@
       </c>
       <c r="K92" t="inlineStr">
         <is>
-          <t>Processes for acquiring vulnerability information, identification, evaluation, testing, and deployment of patches described; PEN-testing and vulnerability remediation timelines included.</t>
+          <t>Anti-malware controls in place with mandatory antivirus and incident reporting procedures.</t>
         </is>
       </c>
       <c r="L92" t="inlineStr">
@@ -5774,12 +5818,12 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>A.8.9</t>
+          <t>A.8.8</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Configuration management</t>
+          <t>Management of technical vulnerabilities</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -5789,34 +5833,93 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Section 6.3 Configuration Management requires documentation of design and configuration of key IT systems, annual review, and updates upon significant changes. Section 6.9 Network Security Policy includes configuration backup and change logging for network devices.</t>
+          <t>A formal patch management process exists including acquisition of vulnerability information, assessment, testing, and deployment of patches. Subscriptions to vulnerability notifications are maintained.</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>6.3 Configuration Management; 6.9.35 A backup of all networking and security devices managed must be taken before and after any major configuration changes. (Information Security Policy [Internal].docx)</t>
+          <t>Information Security Policy [Internal].docx Section 6.2 Management of technical vulnerabilities; Section 6.5 Security incident management.</t>
         </is>
       </c>
       <c r="H93" t="inlineStr"/>
       <c r="I93" t="inlineStr"/>
       <c r="J93" t="inlineStr">
         <is>
-          <t>No direct evidence found in provided documents.</t>
+          <t>Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
         </is>
       </c>
       <c r="K93" t="inlineStr">
         <is>
-          <t>No explicit configuration management documentation or change logging found.</t>
+          <t>Formal patch management process exists including vulnerability information acquisition and deployment of patches.</t>
         </is>
       </c>
       <c r="L93" t="inlineStr">
         <is>
-          <t>Document configuration management and change logging procedures.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="M93" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>A.8 (Technological Controls)</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>A.8.9</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Configuration management</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>Configuration management documents are maintained, reviewed annually, and updated upon significant changes. Change management processes control changes to systems and configurations.</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>Information Security Policy [Internal].docx Sections 6.3 Configuration Management; 6.2 Operational change control.</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr"/>
+      <c r="I94" t="inlineStr"/>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>Management Review Team Meeting E-WISE 2025 [Restricted].docx.pdf</t>
+        </is>
+      </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>Configuration management documents maintained, reviewed annually; change management controls changes.</t>
+        </is>
+      </c>
+      <c r="L94" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M94" t="inlineStr">
+        <is>
+          <t>✅</t>
         </is>
       </c>
     </row>

</xml_diff>